<commit_message>
20231122: Completed coding for MAB, pending test
</commit_message>
<xml_diff>
--- a/output/fit_clients/fit_round_1.xlsx
+++ b/output/fit_clients/fit_round_1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L101"/>
+  <dimension ref="A1:I101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,52 +441,37 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>cyclePerBit</t>
+          <t>dataSize</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>dataSize</t>
+          <t>frequency</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>frequency</t>
+          <t>transPower</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>transPower</t>
+          <t>updateTime</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>updateTime</t>
+          <t>isSelected</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>bandwidth</t>
+          <t>C</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>transRate</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>uploadTime</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>totalTime</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>isSelected</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -500,33 +485,26 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>131.7035989506647</v>
+        <v>450</v>
       </c>
       <c r="D2" t="n">
-        <v>15488376</v>
+        <v>4631561151.493849</v>
       </c>
       <c r="E2" t="n">
-        <v>1219290287.758446</v>
+        <v>0.001938892638358515</v>
       </c>
       <c r="F2" t="n">
-        <v>0.003192289446770954</v>
-      </c>
-      <c r="G2" t="n">
-        <v>8.365009061341846</v>
+        <v>0.0005655522866528816</v>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
       </c>
       <c r="H2" t="n">
-        <v>50000</v>
+        <v>7.069403583161021e-06</v>
       </c>
       <c r="I2" t="n">
-        <v>59354.04641635028</v>
-      </c>
-      <c r="J2" t="n">
-        <v>33.42976797372005</v>
-      </c>
-      <c r="K2" t="n">
-        <v>41.79477703506189</v>
-      </c>
-      <c r="L2" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -538,33 +516,26 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>129.6377424980137</v>
+        <v>450</v>
       </c>
       <c r="D3" t="n">
-        <v>15784824</v>
+        <v>3215255551.869132</v>
       </c>
       <c r="E3" t="n">
-        <v>165359353.3359599</v>
+        <v>0.004034955675476349</v>
       </c>
       <c r="F3" t="n">
-        <v>0.003864131169786561</v>
-      </c>
-      <c r="G3" t="n">
-        <v>61.87460545189088</v>
+        <v>0.0008146755235294638</v>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
       </c>
       <c r="H3" t="n">
-        <v>50000</v>
+        <v>1.01834440441183e-05</v>
       </c>
       <c r="I3" t="n">
-        <v>67401.77380880335</v>
-      </c>
-      <c r="J3" t="n">
-        <v>29.43827569921972</v>
-      </c>
-      <c r="K3" t="n">
-        <v>91.3128811511106</v>
-      </c>
-      <c r="L3" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -576,34 +547,25 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>68.34480074296896</v>
+        <v>450</v>
       </c>
       <c r="D4" t="n">
-        <v>16097144</v>
+        <v>1914563032.738912</v>
       </c>
       <c r="E4" t="n">
-        <v>1749996524.930049</v>
+        <v>0.001761175115914675</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0009252013217896581</v>
-      </c>
-      <c r="G4" t="n">
-        <v>3.143309382442499</v>
+        <v>0.001368139860223241</v>
+      </c>
+      <c r="G4" t="b">
+        <v>1</v>
       </c>
       <c r="H4" t="n">
-        <v>50000</v>
+        <v>1.710174825279052e-05</v>
       </c>
       <c r="I4" t="n">
-        <v>22713.03462150439</v>
-      </c>
-      <c r="J4" t="n">
-        <v>87.35917648456338</v>
-      </c>
-      <c r="K4" t="n">
-        <v>90.50248586700587</v>
-      </c>
-      <c r="L4" t="b">
-        <v>1</v>
+        <v>450</v>
       </c>
     </row>
     <row r="5">
@@ -616,34 +578,25 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>70.0811743466289</v>
+        <v>450</v>
       </c>
       <c r="D5" t="n">
-        <v>15614840</v>
+        <v>4494078122.686357</v>
       </c>
       <c r="E5" t="n">
-        <v>455214976.127611</v>
+        <v>0.003808431903850573</v>
       </c>
       <c r="F5" t="n">
-        <v>0.004418094305063257</v>
-      </c>
-      <c r="G5" t="n">
-        <v>12.01966523315729</v>
+        <v>0.0005828536862270313</v>
+      </c>
+      <c r="G5" t="b">
+        <v>1</v>
       </c>
       <c r="H5" t="n">
-        <v>50000</v>
+        <v>7.285671077837891e-06</v>
       </c>
       <c r="I5" t="n">
-        <v>73422.32926380888</v>
-      </c>
-      <c r="J5" t="n">
-        <v>27.02436738108283</v>
-      </c>
-      <c r="K5" t="n">
-        <v>39.04403261424012</v>
-      </c>
-      <c r="L5" t="b">
-        <v>1</v>
+        <v>450</v>
       </c>
     </row>
     <row r="6">
@@ -656,34 +609,25 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>194.2372859940591</v>
+        <v>450</v>
       </c>
       <c r="D6" t="n">
-        <v>16079736</v>
+        <v>649032361.169804</v>
       </c>
       <c r="E6" t="n">
-        <v>494094943.2862005</v>
+        <v>0.00150975763253524</v>
       </c>
       <c r="F6" t="n">
-        <v>0.004650925389920485</v>
-      </c>
-      <c r="G6" t="n">
-        <v>31.60611459983948</v>
+        <v>0.004035838822087175</v>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
       </c>
       <c r="H6" t="n">
-        <v>50000</v>
+        <v>5.044798527608969e-05</v>
       </c>
       <c r="I6" t="n">
-        <v>75810.09279816743</v>
-      </c>
-      <c r="J6" t="n">
-        <v>26.17319049170144</v>
-      </c>
-      <c r="K6" t="n">
-        <v>57.77930509154092</v>
-      </c>
-      <c r="L6" t="b">
-        <v>1</v>
+        <v>450</v>
       </c>
     </row>
     <row r="7">
@@ -696,33 +640,26 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>164.0057935520288</v>
+        <v>450</v>
       </c>
       <c r="D7" t="n">
-        <v>16201080</v>
+        <v>1439398421.84168</v>
       </c>
       <c r="E7" t="n">
-        <v>253423766.9691948</v>
+        <v>0.001124963951718809</v>
       </c>
       <c r="F7" t="n">
-        <v>0.004470699359474977</v>
-      </c>
-      <c r="G7" t="n">
-        <v>52.42347656608871</v>
+        <v>0.001819781069822591</v>
+      </c>
+      <c r="G7" t="b">
+        <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>50000</v>
+        <v>2.274726337278238e-05</v>
       </c>
       <c r="I7" t="n">
-        <v>73968.76559138448</v>
-      </c>
-      <c r="J7" t="n">
-        <v>26.8247277636212</v>
-      </c>
-      <c r="K7" t="n">
-        <v>79.24820432970992</v>
-      </c>
-      <c r="L7" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -734,33 +671,26 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>131.2969929818012</v>
+        <v>450</v>
       </c>
       <c r="D8" t="n">
-        <v>16060792</v>
+        <v>2429573859.261202</v>
       </c>
       <c r="E8" t="n">
-        <v>912338908.2604424</v>
+        <v>0.004399902958873724</v>
       </c>
       <c r="F8" t="n">
-        <v>0.003012638031732604</v>
-      </c>
-      <c r="G8" t="n">
-        <v>11.55674539041031</v>
+        <v>0.001078127339086748</v>
+      </c>
+      <c r="G8" t="b">
+        <v>1</v>
       </c>
       <c r="H8" t="n">
-        <v>50000</v>
+        <v>1.347659173858434e-05</v>
       </c>
       <c r="I8" t="n">
-        <v>57040.73900413276</v>
-      </c>
-      <c r="J8" t="n">
-        <v>34.78552407703273</v>
-      </c>
-      <c r="K8" t="n">
-        <v>46.34226946744303</v>
-      </c>
-      <c r="L8" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -772,33 +702,26 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>131.771643408771</v>
+        <v>450</v>
       </c>
       <c r="D9" t="n">
-        <v>15906680</v>
+        <v>128668985.2499559</v>
       </c>
       <c r="E9" t="n">
-        <v>1988854766.990456</v>
+        <v>0.003685636824709343</v>
       </c>
       <c r="F9" t="n">
-        <v>0.0005700340358419018</v>
-      </c>
-      <c r="G9" t="n">
-        <v>5.269488249132391</v>
+        <v>0.02035758652259129</v>
+      </c>
+      <c r="G9" t="b">
+        <v>1</v>
       </c>
       <c r="H9" t="n">
-        <v>50000</v>
+        <v>0.0002544698315323911</v>
       </c>
       <c r="I9" t="n">
-        <v>14816.3277596413</v>
-      </c>
-      <c r="J9" t="n">
-        <v>133.9192836571021</v>
-      </c>
-      <c r="K9" t="n">
-        <v>139.1887719062345</v>
-      </c>
-      <c r="L9" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -810,33 +733,26 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>80.74018507938591</v>
+        <v>450</v>
       </c>
       <c r="D10" t="n">
-        <v>15889784</v>
+        <v>678282383.9485012</v>
       </c>
       <c r="E10" t="n">
-        <v>516504452.7799202</v>
+        <v>0.003095855959157138</v>
       </c>
       <c r="F10" t="n">
-        <v>0.001414322403643372</v>
-      </c>
-      <c r="G10" t="n">
-        <v>12.41948732606687</v>
+        <v>0.003861798657885943</v>
+      </c>
+      <c r="G10" t="b">
+        <v>1</v>
       </c>
       <c r="H10" t="n">
-        <v>50000</v>
+        <v>4.827248322357429e-05</v>
       </c>
       <c r="I10" t="n">
-        <v>32341.72468623463</v>
-      </c>
-      <c r="J10" t="n">
-        <v>61.35084072509333</v>
-      </c>
-      <c r="K10" t="n">
-        <v>73.77032805116021</v>
-      </c>
-      <c r="L10" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -848,33 +764,26 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>175.3657314424443</v>
+        <v>450</v>
       </c>
       <c r="D11" t="n">
-        <v>16133496</v>
+        <v>1824765719.917668</v>
       </c>
       <c r="E11" t="n">
-        <v>1239794877.991666</v>
+        <v>0.000812304082011366</v>
       </c>
       <c r="F11" t="n">
-        <v>0.002099552762864036</v>
-      </c>
-      <c r="G11" t="n">
-        <v>11.41020332067692</v>
+        <v>0.00143546646641202</v>
+      </c>
+      <c r="G11" t="b">
+        <v>1</v>
       </c>
       <c r="H11" t="n">
-        <v>50000</v>
+        <v>1.794333083015025e-05</v>
       </c>
       <c r="I11" t="n">
-        <v>43978.27463839236</v>
-      </c>
-      <c r="J11" t="n">
-        <v>45.11754988832215</v>
-      </c>
-      <c r="K11" t="n">
-        <v>56.52775320899907</v>
-      </c>
-      <c r="L11" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -886,33 +795,26 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>138.5972138656425</v>
+        <v>450</v>
       </c>
       <c r="D12" t="n">
-        <v>15558520</v>
+        <v>3712068996.921957</v>
       </c>
       <c r="E12" t="n">
-        <v>1554519571.660179</v>
+        <v>0.001846419463877546</v>
       </c>
       <c r="F12" t="n">
-        <v>0.001545443263640773</v>
-      </c>
-      <c r="G12" t="n">
-        <v>6.935800498059804</v>
+        <v>0.0007056415174857998</v>
+      </c>
+      <c r="G12" t="b">
+        <v>1</v>
       </c>
       <c r="H12" t="n">
-        <v>50000</v>
+        <v>8.820518968572498e-06</v>
       </c>
       <c r="I12" t="n">
-        <v>34718.48470508213</v>
-      </c>
-      <c r="J12" t="n">
-        <v>57.15088134908007</v>
-      </c>
-      <c r="K12" t="n">
-        <v>64.08668184713987</v>
-      </c>
-      <c r="L12" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -924,34 +826,25 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>115.3831562097979</v>
+        <v>450</v>
       </c>
       <c r="D13" t="n">
-        <v>15959928</v>
+        <v>2641715195.622495</v>
       </c>
       <c r="E13" t="n">
-        <v>1683752465.822439</v>
+        <v>0.001771264182260648</v>
       </c>
       <c r="F13" t="n">
-        <v>0.004345642393387241</v>
-      </c>
-      <c r="G13" t="n">
-        <v>5.468460782985794</v>
+        <v>0.0009915489770965891</v>
+      </c>
+      <c r="G13" t="b">
+        <v>1</v>
       </c>
       <c r="H13" t="n">
-        <v>50000</v>
+        <v>1.239436221370736e-05</v>
       </c>
       <c r="I13" t="n">
-        <v>72662.89175468773</v>
-      </c>
-      <c r="J13" t="n">
-        <v>27.30681303874743</v>
-      </c>
-      <c r="K13" t="n">
-        <v>32.77527382173322</v>
-      </c>
-      <c r="L13" t="b">
-        <v>1</v>
+        <v>450</v>
       </c>
     </row>
     <row r="14">
@@ -964,33 +857,26 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>50.73295897686648</v>
+        <v>450</v>
       </c>
       <c r="D14" t="n">
-        <v>15532920</v>
+        <v>4421137649.298481</v>
       </c>
       <c r="E14" t="n">
-        <v>1235457484.419105</v>
+        <v>0.003452755306270073</v>
       </c>
       <c r="F14" t="n">
-        <v>0.004987517010978175</v>
-      </c>
-      <c r="G14" t="n">
-        <v>3.189227484916126</v>
+        <v>0.0005924696781190762</v>
+      </c>
+      <c r="G14" t="b">
+        <v>1</v>
       </c>
       <c r="H14" t="n">
-        <v>50000</v>
+        <v>7.405870976488452e-06</v>
       </c>
       <c r="I14" t="n">
-        <v>79127.96403468285</v>
-      </c>
-      <c r="J14" t="n">
-        <v>25.07573680437806</v>
-      </c>
-      <c r="K14" t="n">
-        <v>28.26496428929418</v>
-      </c>
-      <c r="L14" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -1002,34 +888,25 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>101.5332290424106</v>
+        <v>450</v>
       </c>
       <c r="D15" t="n">
-        <v>16140152</v>
+        <v>472000757.0176398</v>
       </c>
       <c r="E15" t="n">
-        <v>972343667.9797889</v>
+        <v>0.003634701069172503</v>
       </c>
       <c r="F15" t="n">
-        <v>0.004364473150747446</v>
-      </c>
-      <c r="G15" t="n">
-        <v>8.426864923181585</v>
+        <v>0.005549546184100944</v>
+      </c>
+      <c r="G15" t="b">
+        <v>1</v>
       </c>
       <c r="H15" t="n">
-        <v>50000</v>
+        <v>6.936932730126181e-05</v>
       </c>
       <c r="I15" t="n">
-        <v>72861.04513461892</v>
-      </c>
-      <c r="J15" t="n">
-        <v>27.23254924951987</v>
-      </c>
-      <c r="K15" t="n">
-        <v>35.65941417270145</v>
-      </c>
-      <c r="L15" t="b">
-        <v>1</v>
+        <v>450</v>
       </c>
     </row>
     <row r="16">
@@ -1042,33 +919,26 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>95.02341235901179</v>
+        <v>450</v>
       </c>
       <c r="D16" t="n">
-        <v>16104312</v>
+        <v>1590104679.135227</v>
       </c>
       <c r="E16" t="n">
-        <v>1341661484.792166</v>
+        <v>0.001000698564808018</v>
       </c>
       <c r="F16" t="n">
-        <v>0.003068509979461345</v>
-      </c>
-      <c r="G16" t="n">
-        <v>5.702953752791211</v>
+        <v>0.001647306642368064</v>
+      </c>
+      <c r="G16" t="b">
+        <v>1</v>
       </c>
       <c r="H16" t="n">
-        <v>50000</v>
+        <v>2.05913330296008e-05</v>
       </c>
       <c r="I16" t="n">
-        <v>57768.16241650885</v>
-      </c>
-      <c r="J16" t="n">
-        <v>34.34750071663976</v>
-      </c>
-      <c r="K16" t="n">
-        <v>40.05045446943097</v>
-      </c>
-      <c r="L16" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -1080,33 +950,26 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>143.9265239644386</v>
+        <v>450</v>
       </c>
       <c r="D17" t="n">
-        <v>15844728</v>
+        <v>2923716675.120843</v>
       </c>
       <c r="E17" t="n">
-        <v>1386083317.943482</v>
+        <v>0.00443580115018765</v>
       </c>
       <c r="F17" t="n">
-        <v>0.00281757807231493</v>
-      </c>
-      <c r="G17" t="n">
-        <v>8.226333131205752</v>
+        <v>0.0008959110238996518</v>
+      </c>
+      <c r="G17" t="b">
+        <v>1</v>
       </c>
       <c r="H17" t="n">
-        <v>50000</v>
+        <v>1.119888779874565e-05</v>
       </c>
       <c r="I17" t="n">
-        <v>54442.06075016414</v>
-      </c>
-      <c r="J17" t="n">
-        <v>36.44593853832063</v>
-      </c>
-      <c r="K17" t="n">
-        <v>44.67227166952638</v>
-      </c>
-      <c r="L17" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -1118,33 +981,26 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>147.1204516209924</v>
+        <v>450</v>
       </c>
       <c r="D18" t="n">
-        <v>15865208</v>
+        <v>3159157060.400885</v>
       </c>
       <c r="E18" t="n">
-        <v>1177153930.869146</v>
+        <v>0.00474565561140208</v>
       </c>
       <c r="F18" t="n">
-        <v>0.001772915652039073</v>
-      </c>
-      <c r="G18" t="n">
-        <v>9.914151857342956</v>
+        <v>0.0008291420622397323</v>
+      </c>
+      <c r="G18" t="b">
+        <v>1</v>
       </c>
       <c r="H18" t="n">
-        <v>50000</v>
+        <v>1.036427577799665e-05</v>
       </c>
       <c r="I18" t="n">
-        <v>38664.63717040241</v>
-      </c>
-      <c r="J18" t="n">
-        <v>51.31800387147793</v>
-      </c>
-      <c r="K18" t="n">
-        <v>61.23215572882089</v>
-      </c>
-      <c r="L18" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -1156,33 +1012,26 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>51.0740668709074</v>
+        <v>450</v>
       </c>
       <c r="D19" t="n">
-        <v>15872888</v>
+        <v>2651005561.576064</v>
       </c>
       <c r="E19" t="n">
-        <v>987672733.2859198</v>
+        <v>0.002338189809745013</v>
       </c>
       <c r="F19" t="n">
-        <v>0.003707351769117449</v>
-      </c>
-      <c r="G19" t="n">
-        <v>4.10405651500221</v>
+        <v>0.0009880741247644657</v>
+      </c>
+      <c r="G19" t="b">
+        <v>1</v>
       </c>
       <c r="H19" t="n">
-        <v>50000</v>
+        <v>1.235092655955582e-05</v>
       </c>
       <c r="I19" t="n">
-        <v>65602.49052630132</v>
-      </c>
-      <c r="J19" t="n">
-        <v>30.24568098073195</v>
-      </c>
-      <c r="K19" t="n">
-        <v>34.34973749573416</v>
-      </c>
-      <c r="L19" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -1194,34 +1043,25 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>77.09051986670525</v>
+        <v>450</v>
       </c>
       <c r="D20" t="n">
-        <v>15830392</v>
+        <v>4952709980.820808</v>
       </c>
       <c r="E20" t="n">
-        <v>1623172685.333032</v>
+        <v>0.001143123273030613</v>
       </c>
       <c r="F20" t="n">
-        <v>0.002397388643171247</v>
-      </c>
-      <c r="G20" t="n">
-        <v>3.759221554185233</v>
+        <v>0.0005288801504920525</v>
+      </c>
+      <c r="G20" t="b">
+        <v>1</v>
       </c>
       <c r="H20" t="n">
-        <v>50000</v>
+        <v>6.611001881150657e-06</v>
       </c>
       <c r="I20" t="n">
-        <v>48504.22969884496</v>
-      </c>
-      <c r="J20" t="n">
-        <v>40.90760769358739</v>
-      </c>
-      <c r="K20" t="n">
-        <v>44.66682924777262</v>
-      </c>
-      <c r="L20" t="b">
-        <v>1</v>
+        <v>450</v>
       </c>
     </row>
     <row r="21">
@@ -1234,33 +1074,26 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>109.0660310813776</v>
+        <v>450</v>
       </c>
       <c r="D21" t="n">
-        <v>16203640</v>
+        <v>3792716796.773875</v>
       </c>
       <c r="E21" t="n">
-        <v>1179922472.422218</v>
+        <v>0.0006432460950695578</v>
       </c>
       <c r="F21" t="n">
-        <v>0.0008188342993723406</v>
-      </c>
-      <c r="G21" t="n">
-        <v>7.488910268161511</v>
+        <v>0.0006906368548867348</v>
+      </c>
+      <c r="G21" t="b">
+        <v>1</v>
       </c>
       <c r="H21" t="n">
-        <v>50000</v>
+        <v>8.632960686084184e-06</v>
       </c>
       <c r="I21" t="n">
-        <v>20437.42531876851</v>
-      </c>
-      <c r="J21" t="n">
-        <v>97.08620186016466</v>
-      </c>
-      <c r="K21" t="n">
-        <v>104.5751121283262</v>
-      </c>
-      <c r="L21" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -1272,33 +1105,26 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>96.07512658262159</v>
+        <v>450</v>
       </c>
       <c r="D22" t="n">
-        <v>15552376</v>
+        <v>128519285.7007198</v>
       </c>
       <c r="E22" t="n">
-        <v>1493740460.761776</v>
+        <v>0.004340489530750181</v>
       </c>
       <c r="F22" t="n">
-        <v>0.002099452956236495</v>
-      </c>
-      <c r="G22" t="n">
-        <v>5.001526477024388</v>
+        <v>0.02038129908455699</v>
+      </c>
+      <c r="G22" t="b">
+        <v>0</v>
       </c>
       <c r="H22" t="n">
-        <v>50000</v>
+        <v>0.0002547662385569624</v>
       </c>
       <c r="I22" t="n">
-        <v>43976.70935480625</v>
-      </c>
-      <c r="J22" t="n">
-        <v>45.11915577837899</v>
-      </c>
-      <c r="K22" t="n">
-        <v>50.12068225540338</v>
-      </c>
-      <c r="L22" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -1310,33 +1136,26 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>170.9372235190259</v>
+        <v>450</v>
       </c>
       <c r="D23" t="n">
-        <v>16007544</v>
+        <v>3328936270.761126</v>
       </c>
       <c r="E23" t="n">
-        <v>1997049464.129853</v>
+        <v>0.001084603850167031</v>
       </c>
       <c r="F23" t="n">
-        <v>0.004245507925643886</v>
-      </c>
-      <c r="G23" t="n">
-        <v>6.850819611298125</v>
+        <v>0.0007868549551419032</v>
+      </c>
+      <c r="G23" t="b">
+        <v>0</v>
       </c>
       <c r="H23" t="n">
-        <v>50000</v>
+        <v>9.83568693927379e-06</v>
       </c>
       <c r="I23" t="n">
-        <v>71599.9492469128</v>
-      </c>
-      <c r="J23" t="n">
-        <v>27.71219841451987</v>
-      </c>
-      <c r="K23" t="n">
-        <v>34.563018025818</v>
-      </c>
-      <c r="L23" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -1348,33 +1167,26 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>185.210834924772</v>
+        <v>450</v>
       </c>
       <c r="D24" t="n">
-        <v>15793016</v>
+        <v>381062351.8244779</v>
       </c>
       <c r="E24" t="n">
-        <v>1145275092.955674</v>
+        <v>0.000841316538259083</v>
       </c>
       <c r="F24" t="n">
-        <v>0.003841994255060609</v>
-      </c>
-      <c r="G24" t="n">
-        <v>12.77002223016777</v>
+        <v>0.006873914432792153</v>
+      </c>
+      <c r="G24" t="b">
+        <v>0</v>
       </c>
       <c r="H24" t="n">
-        <v>50000</v>
+        <v>8.592393040990191e-05</v>
       </c>
       <c r="I24" t="n">
-        <v>67150.42378398468</v>
-      </c>
-      <c r="J24" t="n">
-        <v>29.54846579052012</v>
-      </c>
-      <c r="K24" t="n">
-        <v>42.31848802068789</v>
-      </c>
-      <c r="L24" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -1386,33 +1198,26 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>136.3881723406921</v>
+        <v>450</v>
       </c>
       <c r="D25" t="n">
-        <v>15961976</v>
+        <v>4270985989.805146</v>
       </c>
       <c r="E25" t="n">
-        <v>640677758.7324127</v>
+        <v>0.0009375163623674614</v>
       </c>
       <c r="F25" t="n">
-        <v>0.004955492020819411</v>
-      </c>
-      <c r="G25" t="n">
-        <v>16.9900133406633</v>
+        <v>0.0006132986636464016</v>
+      </c>
+      <c r="G25" t="b">
+        <v>0</v>
       </c>
       <c r="H25" t="n">
-        <v>50000</v>
+        <v>7.666233295580019e-06</v>
       </c>
       <c r="I25" t="n">
-        <v>78818.77352877437</v>
-      </c>
-      <c r="J25" t="n">
-        <v>25.17410397505908</v>
-      </c>
-      <c r="K25" t="n">
-        <v>42.16411731572238</v>
-      </c>
-      <c r="L25" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -1424,33 +1229,26 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>170.3461580119232</v>
+        <v>450</v>
       </c>
       <c r="D26" t="n">
-        <v>16193912</v>
+        <v>1992078431.92715</v>
       </c>
       <c r="E26" t="n">
-        <v>474775265.6961866</v>
+        <v>0.0009962347500754025</v>
       </c>
       <c r="F26" t="n">
-        <v>0.003042907793750083</v>
-      </c>
-      <c r="G26" t="n">
-        <v>29.05133114230529</v>
+        <v>0.001314903046997996</v>
+      </c>
+      <c r="G26" t="b">
+        <v>0</v>
       </c>
       <c r="H26" t="n">
-        <v>50000</v>
+        <v>1.643628808747495e-05</v>
       </c>
       <c r="I26" t="n">
-        <v>57435.74568553287</v>
-      </c>
-      <c r="J26" t="n">
-        <v>34.54629127414264</v>
-      </c>
-      <c r="K26" t="n">
-        <v>63.59762241644793</v>
-      </c>
-      <c r="L26" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -1462,33 +1260,26 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>159.2079430866664</v>
+        <v>450</v>
       </c>
       <c r="D27" t="n">
-        <v>16001912</v>
+        <v>4193882394.649139</v>
       </c>
       <c r="E27" t="n">
-        <v>614993506.2753246</v>
+        <v>0.003494035630699183</v>
       </c>
       <c r="F27" t="n">
-        <v>0.004815864622757536</v>
-      </c>
-      <c r="G27" t="n">
-        <v>20.71266988169874</v>
+        <v>0.0006245740231872045</v>
+      </c>
+      <c r="G27" t="b">
+        <v>0</v>
       </c>
       <c r="H27" t="n">
-        <v>50000</v>
+        <v>7.807175289840055e-06</v>
       </c>
       <c r="I27" t="n">
-        <v>77455.01419665423</v>
-      </c>
-      <c r="J27" t="n">
-        <v>25.61734731546547</v>
-      </c>
-      <c r="K27" t="n">
-        <v>46.33001719716421</v>
-      </c>
-      <c r="L27" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -1500,33 +1291,26 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>138.0938849503207</v>
+        <v>450</v>
       </c>
       <c r="D28" t="n">
-        <v>15453048</v>
+        <v>2722322212.960444</v>
       </c>
       <c r="E28" t="n">
-        <v>1218011359.352355</v>
+        <v>0.001329494710253971</v>
       </c>
       <c r="F28" t="n">
-        <v>0.003757638422977768</v>
-      </c>
-      <c r="G28" t="n">
-        <v>8.760063755803008</v>
+        <v>0.0009621895554940542</v>
+      </c>
+      <c r="G28" t="b">
+        <v>0</v>
       </c>
       <c r="H28" t="n">
-        <v>50000</v>
+        <v>1.202736944367568e-05</v>
       </c>
       <c r="I28" t="n">
-        <v>66184.51023596892</v>
-      </c>
-      <c r="J28" t="n">
-        <v>29.97970360324073</v>
-      </c>
-      <c r="K28" t="n">
-        <v>38.73976735904373</v>
-      </c>
-      <c r="L28" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -1538,33 +1322,26 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>115.6152507552942</v>
+        <v>450</v>
       </c>
       <c r="D29" t="n">
-        <v>15797624</v>
+        <v>703231843.1428608</v>
       </c>
       <c r="E29" t="n">
-        <v>742742248.5512544</v>
+        <v>0.002081391905835109</v>
       </c>
       <c r="F29" t="n">
-        <v>0.001065084204149732</v>
-      </c>
-      <c r="G29" t="n">
-        <v>12.29528994520241</v>
+        <v>0.003724788667551668</v>
+      </c>
+      <c r="G29" t="b">
+        <v>0</v>
       </c>
       <c r="H29" t="n">
-        <v>50000</v>
+        <v>4.655985834439585e-05</v>
       </c>
       <c r="I29" t="n">
-        <v>25600.40286853736</v>
-      </c>
-      <c r="J29" t="n">
-        <v>77.50628027961825</v>
-      </c>
-      <c r="K29" t="n">
-        <v>89.80157022482067</v>
-      </c>
-      <c r="L29" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -1576,33 +1353,26 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>199.5061061252951</v>
+        <v>450</v>
       </c>
       <c r="D30" t="n">
-        <v>15640952</v>
+        <v>2651743904.544246</v>
       </c>
       <c r="E30" t="n">
-        <v>881324288.1421239</v>
+        <v>0.004898620322817088</v>
       </c>
       <c r="F30" t="n">
-        <v>0.001003601642256517</v>
-      </c>
-      <c r="G30" t="n">
-        <v>17.70327603356277</v>
+        <v>0.0009877990086113511</v>
+      </c>
+      <c r="G30" t="b">
+        <v>0</v>
       </c>
       <c r="H30" t="n">
-        <v>50000</v>
+        <v>1.234748760764189e-05</v>
       </c>
       <c r="I30" t="n">
-        <v>24345.53278381005</v>
-      </c>
-      <c r="J30" t="n">
-        <v>81.50127654300101</v>
-      </c>
-      <c r="K30" t="n">
-        <v>99.20455257656378</v>
-      </c>
-      <c r="L30" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -1614,33 +1384,26 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>76.7803339559247</v>
+        <v>450</v>
       </c>
       <c r="D31" t="n">
-        <v>16222072</v>
+        <v>4401565284.951936</v>
       </c>
       <c r="E31" t="n">
-        <v>376702764.5959192</v>
+        <v>0.003326939142700229</v>
       </c>
       <c r="F31" t="n">
-        <v>0.001807422282938164</v>
-      </c>
-      <c r="G31" t="n">
-        <v>16.53208076337208</v>
+        <v>0.0005951042028060259</v>
+      </c>
+      <c r="G31" t="b">
+        <v>0</v>
       </c>
       <c r="H31" t="n">
-        <v>50000</v>
+        <v>7.438802535075324e-06</v>
       </c>
       <c r="I31" t="n">
-        <v>39244.83359200048</v>
-      </c>
-      <c r="J31" t="n">
-        <v>50.55931745381258</v>
-      </c>
-      <c r="K31" t="n">
-        <v>67.09139821718466</v>
-      </c>
-      <c r="L31" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -1652,34 +1415,25 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>94.581449557051</v>
+        <v>450</v>
       </c>
       <c r="D32" t="n">
-        <v>15745912</v>
+        <v>1638027954.409359</v>
       </c>
       <c r="E32" t="n">
-        <v>1199323424.72726</v>
+        <v>0.001537645572784908</v>
       </c>
       <c r="F32" t="n">
-        <v>0.0035075620188395</v>
-      </c>
-      <c r="G32" t="n">
-        <v>6.208797188700125</v>
+        <v>0.001599111903401246</v>
+      </c>
+      <c r="G32" t="b">
+        <v>0</v>
       </c>
       <c r="H32" t="n">
-        <v>50000</v>
+        <v>1.998889879251557e-05</v>
       </c>
       <c r="I32" t="n">
-        <v>63242.57710761989</v>
-      </c>
-      <c r="J32" t="n">
-        <v>31.37430653123924</v>
-      </c>
-      <c r="K32" t="n">
-        <v>37.58310371993937</v>
-      </c>
-      <c r="L32" t="b">
-        <v>1</v>
+        <v>450</v>
       </c>
     </row>
     <row r="33">
@@ -1692,33 +1446,26 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>199.5192821624728</v>
+        <v>450</v>
       </c>
       <c r="D33" t="n">
-        <v>15923064</v>
+        <v>335125820.7473602</v>
       </c>
       <c r="E33" t="n">
-        <v>403316599.3109738</v>
+        <v>0.0005005090786617887</v>
       </c>
       <c r="F33" t="n">
-        <v>0.004251695102803425</v>
-      </c>
-      <c r="G33" t="n">
-        <v>39.38541464118546</v>
+        <v>0.007816139007607735</v>
+      </c>
+      <c r="G33" t="b">
+        <v>0</v>
       </c>
       <c r="H33" t="n">
-        <v>50000</v>
+        <v>9.770173759509669e-05</v>
       </c>
       <c r="I33" t="n">
-        <v>71666.08302597496</v>
-      </c>
-      <c r="J33" t="n">
-        <v>27.68662547499409</v>
-      </c>
-      <c r="K33" t="n">
-        <v>67.07204011617955</v>
-      </c>
-      <c r="L33" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -1730,34 +1477,25 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>174.7403450780672</v>
+        <v>450</v>
       </c>
       <c r="D34" t="n">
-        <v>15801720</v>
+        <v>2512925982.691546</v>
       </c>
       <c r="E34" t="n">
-        <v>570993734.4123659</v>
+        <v>0.00422366396888548</v>
       </c>
       <c r="F34" t="n">
-        <v>0.001369001697955677</v>
-      </c>
-      <c r="G34" t="n">
-        <v>24.17888182668645</v>
+        <v>0.0010423665551798</v>
+      </c>
+      <c r="G34" t="b">
+        <v>0</v>
       </c>
       <c r="H34" t="n">
-        <v>50000</v>
+        <v>1.302958193974749e-05</v>
       </c>
       <c r="I34" t="n">
-        <v>31501.66335185682</v>
-      </c>
-      <c r="J34" t="n">
-        <v>62.98689621045183</v>
-      </c>
-      <c r="K34" t="n">
-        <v>87.16577803713828</v>
-      </c>
-      <c r="L34" t="b">
-        <v>1</v>
+        <v>450</v>
       </c>
     </row>
     <row r="35">
@@ -1770,33 +1508,26 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>58.94547510177912</v>
+        <v>450</v>
       </c>
       <c r="D35" t="n">
-        <v>15887224</v>
+        <v>463109970.3158004</v>
       </c>
       <c r="E35" t="n">
-        <v>1603783762.648269</v>
+        <v>0.0008675228470349849</v>
       </c>
       <c r="F35" t="n">
-        <v>0.0009396332129412196</v>
-      </c>
-      <c r="G35" t="n">
-        <v>2.919595485809174</v>
+        <v>0.005656086389618875</v>
+      </c>
+      <c r="G35" t="b">
+        <v>0</v>
       </c>
       <c r="H35" t="n">
-        <v>50000</v>
+        <v>7.070107987023594e-05</v>
       </c>
       <c r="I35" t="n">
-        <v>23016.3317856708</v>
-      </c>
-      <c r="J35" t="n">
-        <v>86.20800301615793</v>
-      </c>
-      <c r="K35" t="n">
-        <v>89.1275985019671</v>
-      </c>
-      <c r="L35" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -1808,33 +1539,26 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>194.1691193044101</v>
+        <v>450</v>
       </c>
       <c r="D36" t="n">
-        <v>16485752</v>
+        <v>4592921599.538335</v>
       </c>
       <c r="E36" t="n">
-        <v>1725371408.639686</v>
+        <v>0.002421597028799308</v>
       </c>
       <c r="F36" t="n">
-        <v>0.00201343305101706</v>
-      </c>
-      <c r="G36" t="n">
-        <v>9.276332999613869</v>
+        <v>0.0005703101921581445</v>
+      </c>
+      <c r="G36" t="b">
+        <v>0</v>
       </c>
       <c r="H36" t="n">
-        <v>50000</v>
+        <v>7.128877401976806e-06</v>
       </c>
       <c r="I36" t="n">
-        <v>42614.85563874473</v>
-      </c>
-      <c r="J36" t="n">
-        <v>46.5610400471709</v>
-      </c>
-      <c r="K36" t="n">
-        <v>55.83737304678477</v>
-      </c>
-      <c r="L36" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -1846,33 +1570,26 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>104.7493473827834</v>
+        <v>450</v>
       </c>
       <c r="D37" t="n">
-        <v>15783800</v>
+        <v>1470009023.493147</v>
       </c>
       <c r="E37" t="n">
-        <v>1714847236.423341</v>
+        <v>0.003286525383607157</v>
       </c>
       <c r="F37" t="n">
-        <v>0.0040558483583373</v>
-      </c>
-      <c r="G37" t="n">
-        <v>4.820670652473848</v>
+        <v>0.001781887021193657</v>
+      </c>
+      <c r="G37" t="b">
+        <v>0</v>
       </c>
       <c r="H37" t="n">
-        <v>50000</v>
+        <v>2.227358776492071e-05</v>
       </c>
       <c r="I37" t="n">
-        <v>69542.71946617543</v>
-      </c>
-      <c r="J37" t="n">
-        <v>28.53198746369247</v>
-      </c>
-      <c r="K37" t="n">
-        <v>33.35265811616632</v>
-      </c>
-      <c r="L37" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -1884,33 +1601,26 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>143.3745043622133</v>
+        <v>450</v>
       </c>
       <c r="D38" t="n">
-        <v>15857528</v>
+        <v>3788004136.683301</v>
       </c>
       <c r="E38" t="n">
-        <v>1643648853.881763</v>
+        <v>0.001367976052532208</v>
       </c>
       <c r="F38" t="n">
-        <v>0.001746394381803476</v>
-      </c>
-      <c r="G38" t="n">
-        <v>6.916213314177473</v>
+        <v>0.000691496076953465</v>
+      </c>
+      <c r="G38" t="b">
+        <v>0</v>
       </c>
       <c r="H38" t="n">
-        <v>50000</v>
+        <v>8.643700961918313e-06</v>
       </c>
       <c r="I38" t="n">
-        <v>38215.51360877315</v>
-      </c>
-      <c r="J38" t="n">
-        <v>51.92111298863946</v>
-      </c>
-      <c r="K38" t="n">
-        <v>58.83732630281694</v>
-      </c>
-      <c r="L38" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -1922,33 +1632,26 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>140.0650621426659</v>
+        <v>450</v>
       </c>
       <c r="D39" t="n">
-        <v>15939448</v>
+        <v>1208119670.546403</v>
       </c>
       <c r="E39" t="n">
-        <v>485569988.6241767</v>
+        <v>0.0005897059007540051</v>
       </c>
       <c r="F39" t="n">
-        <v>0.001348409258613726</v>
-      </c>
-      <c r="G39" t="n">
-        <v>22.9890626165506</v>
+        <v>0.002168154417033301</v>
+      </c>
+      <c r="G39" t="b">
+        <v>0</v>
       </c>
       <c r="H39" t="n">
-        <v>50000</v>
+        <v>2.710193021291627e-05</v>
       </c>
       <c r="I39" t="n">
-        <v>31116.70678037033</v>
-      </c>
-      <c r="J39" t="n">
-        <v>63.76613097282223</v>
-      </c>
-      <c r="K39" t="n">
-        <v>86.75519358937282</v>
-      </c>
-      <c r="L39" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -1960,33 +1663,26 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>128.4598192237846</v>
+        <v>450</v>
       </c>
       <c r="D40" t="n">
-        <v>16810360</v>
+        <v>4977344800.472629</v>
       </c>
       <c r="E40" t="n">
-        <v>392671083.1360512</v>
+        <v>0.004677941756631887</v>
       </c>
       <c r="F40" t="n">
-        <v>0.00286365885180614</v>
-      </c>
-      <c r="G40" t="n">
-        <v>27.49700575657795</v>
+        <v>0.0005262625164628485</v>
+      </c>
+      <c r="G40" t="b">
+        <v>0</v>
       </c>
       <c r="H40" t="n">
-        <v>50000</v>
+        <v>6.578281455785606e-06</v>
       </c>
       <c r="I40" t="n">
-        <v>55064.46923129384</v>
-      </c>
-      <c r="J40" t="n">
-        <v>36.03398030889142</v>
-      </c>
-      <c r="K40" t="n">
-        <v>63.53098606546937</v>
-      </c>
-      <c r="L40" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -1998,33 +1694,26 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>192.3836900220557</v>
+        <v>450</v>
       </c>
       <c r="D41" t="n">
-        <v>15779192</v>
+        <v>1741391679.735254</v>
       </c>
       <c r="E41" t="n">
-        <v>623542666.3300785</v>
+        <v>0.001301468293710195</v>
       </c>
       <c r="F41" t="n">
-        <v>0.003332985147055175</v>
-      </c>
-      <c r="G41" t="n">
-        <v>24.34203260214069</v>
+        <v>0.001504193473807242</v>
+      </c>
+      <c r="G41" t="b">
+        <v>0</v>
       </c>
       <c r="H41" t="n">
-        <v>50000</v>
+        <v>1.880241842259053e-05</v>
       </c>
       <c r="I41" t="n">
-        <v>61115.31528160147</v>
-      </c>
-      <c r="J41" t="n">
-        <v>32.46636282341709</v>
-      </c>
-      <c r="K41" t="n">
-        <v>56.80839542555778</v>
-      </c>
-      <c r="L41" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -2036,33 +1725,26 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>144.5702770354515</v>
+        <v>450</v>
       </c>
       <c r="D42" t="n">
-        <v>15945592</v>
+        <v>4012889470.161499</v>
       </c>
       <c r="E42" t="n">
-        <v>176605772.9987278</v>
+        <v>0.0007232069026177758</v>
       </c>
       <c r="F42" t="n">
-        <v>0.003560531989465902</v>
-      </c>
-      <c r="G42" t="n">
-        <v>65.26566526652799</v>
+        <v>0.0006527441185402455</v>
+      </c>
+      <c r="G42" t="b">
+        <v>0</v>
       </c>
       <c r="H42" t="n">
-        <v>50000</v>
+        <v>8.159301481753068e-06</v>
       </c>
       <c r="I42" t="n">
-        <v>63875.81715900871</v>
-      </c>
-      <c r="J42" t="n">
-        <v>31.06327383743161</v>
-      </c>
-      <c r="K42" t="n">
-        <v>96.3289391039596</v>
-      </c>
-      <c r="L42" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -2074,34 +1756,25 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>69.72078805185139</v>
+        <v>450</v>
       </c>
       <c r="D43" t="n">
-        <v>16385400</v>
+        <v>1659278619.147779</v>
       </c>
       <c r="E43" t="n">
-        <v>331967367.1745522</v>
+        <v>0.001180145356046854</v>
       </c>
       <c r="F43" t="n">
-        <v>0.001038365769593645</v>
-      </c>
-      <c r="G43" t="n">
-        <v>17.20655572666751</v>
+        <v>0.001578631804069978</v>
+      </c>
+      <c r="G43" t="b">
+        <v>0</v>
       </c>
       <c r="H43" t="n">
-        <v>50000</v>
+        <v>1.973289755087472e-05</v>
       </c>
       <c r="I43" t="n">
-        <v>25057.75478965934</v>
-      </c>
-      <c r="J43" t="n">
-        <v>79.18474806125978</v>
-      </c>
-      <c r="K43" t="n">
-        <v>96.3913037879273</v>
-      </c>
-      <c r="L43" t="b">
-        <v>1</v>
+        <v>450</v>
       </c>
     </row>
     <row r="44">
@@ -2114,33 +1787,26 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>98.81571398071829</v>
+        <v>450</v>
       </c>
       <c r="D44" t="n">
-        <v>15893368</v>
+        <v>3462762376.054428</v>
       </c>
       <c r="E44" t="n">
-        <v>919711324.2944291</v>
+        <v>0.0006504033577731836</v>
       </c>
       <c r="F44" t="n">
-        <v>0.003337443953014133</v>
-      </c>
-      <c r="G44" t="n">
-        <v>8.53808398892525</v>
+        <v>0.0007564452063224186</v>
+      </c>
+      <c r="G44" t="b">
+        <v>0</v>
       </c>
       <c r="H44" t="n">
-        <v>50000</v>
+        <v>9.455565079030233e-06</v>
       </c>
       <c r="I44" t="n">
-        <v>61170.43491347713</v>
-      </c>
-      <c r="J44" t="n">
-        <v>32.437107939588</v>
-      </c>
-      <c r="K44" t="n">
-        <v>40.97519192851325</v>
-      </c>
-      <c r="L44" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -2152,33 +1818,26 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>140.4015476322346</v>
+        <v>450</v>
       </c>
       <c r="D45" t="n">
-        <v>15883640</v>
+        <v>4748089150.962017</v>
       </c>
       <c r="E45" t="n">
-        <v>1247699988.47129</v>
+        <v>0.00101477585910925</v>
       </c>
       <c r="F45" t="n">
-        <v>0.002079637999020384</v>
-      </c>
-      <c r="G45" t="n">
-        <v>8.936794336135318</v>
+        <v>0.0005516724553222178</v>
+      </c>
+      <c r="G45" t="b">
+        <v>0</v>
       </c>
       <c r="H45" t="n">
-        <v>50000</v>
+        <v>6.895905691527722e-06</v>
       </c>
       <c r="I45" t="n">
-        <v>43665.27345057857</v>
-      </c>
-      <c r="J45" t="n">
-        <v>45.4409612766025</v>
-      </c>
-      <c r="K45" t="n">
-        <v>54.37775561273781</v>
-      </c>
-      <c r="L45" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -2190,34 +1849,25 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>104.1171544437561</v>
+        <v>450</v>
       </c>
       <c r="D46" t="n">
-        <v>15885176</v>
+        <v>3620875686.984382</v>
       </c>
       <c r="E46" t="n">
-        <v>765437779.3710597</v>
+        <v>0.001103250198622601</v>
       </c>
       <c r="F46" t="n">
-        <v>0.003658695799973893</v>
-      </c>
-      <c r="G46" t="n">
-        <v>10.80374765612713</v>
+        <v>0.0007234134022926201</v>
+      </c>
+      <c r="G46" t="b">
+        <v>0</v>
       </c>
       <c r="H46" t="n">
-        <v>50000</v>
+        <v>9.042667528657752e-06</v>
       </c>
       <c r="I46" t="n">
-        <v>65034.83875844999</v>
-      </c>
-      <c r="J46" t="n">
-        <v>30.50967816449293</v>
-      </c>
-      <c r="K46" t="n">
-        <v>41.31342582062005</v>
-      </c>
-      <c r="L46" t="b">
-        <v>1</v>
+        <v>450</v>
       </c>
     </row>
     <row r="47">
@@ -2230,33 +1880,26 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>179.2742574406265</v>
+        <v>450</v>
       </c>
       <c r="D47" t="n">
-        <v>16013688</v>
+        <v>253949194.421731</v>
       </c>
       <c r="E47" t="n">
-        <v>969547250.9588203</v>
+        <v>0.004984447528964988</v>
       </c>
       <c r="F47" t="n">
-        <v>0.003706517828448244</v>
-      </c>
-      <c r="G47" t="n">
-        <v>14.80506505612177</v>
+        <v>0.01031462220608585</v>
+      </c>
+      <c r="G47" t="b">
+        <v>0</v>
       </c>
       <c r="H47" t="n">
-        <v>50000</v>
+        <v>0.0001289327775760731</v>
       </c>
       <c r="I47" t="n">
-        <v>65592.79876934987</v>
-      </c>
-      <c r="J47" t="n">
-        <v>30.25014997419459</v>
-      </c>
-      <c r="K47" t="n">
-        <v>45.05521503031635</v>
-      </c>
-      <c r="L47" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -2268,33 +1911,26 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>156.1122634922833</v>
+        <v>450</v>
       </c>
       <c r="D48" t="n">
-        <v>16201592</v>
+        <v>1710334872.429317</v>
       </c>
       <c r="E48" t="n">
-        <v>1035182105.694225</v>
+        <v>0.001695047642757514</v>
       </c>
       <c r="F48" t="n">
-        <v>0.002953026274598773</v>
-      </c>
-      <c r="G48" t="n">
-        <v>12.21653265346132</v>
+        <v>0.001531507099705851</v>
+      </c>
+      <c r="G48" t="b">
+        <v>0</v>
       </c>
       <c r="H48" t="n">
-        <v>50000</v>
+        <v>1.914383874632313e-05</v>
       </c>
       <c r="I48" t="n">
-        <v>56256.45059993837</v>
-      </c>
-      <c r="J48" t="n">
-        <v>35.27047971992342</v>
-      </c>
-      <c r="K48" t="n">
-        <v>47.48701237338474</v>
-      </c>
-      <c r="L48" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -2306,33 +1942,26 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>118.4760701063351</v>
+        <v>450</v>
       </c>
       <c r="D49" t="n">
-        <v>16398200</v>
+        <v>2534992985.760207</v>
       </c>
       <c r="E49" t="n">
-        <v>1543971814.478119</v>
+        <v>0.004970094567237064</v>
       </c>
       <c r="F49" t="n">
-        <v>0.002313478220838992</v>
-      </c>
-      <c r="G49" t="n">
-        <v>6.291547146779984</v>
+        <v>0.001033292799906696</v>
+      </c>
+      <c r="G49" t="b">
+        <v>0</v>
       </c>
       <c r="H49" t="n">
-        <v>50000</v>
+        <v>1.29161599988337e-05</v>
       </c>
       <c r="I49" t="n">
-        <v>47257.58339105461</v>
-      </c>
-      <c r="J49" t="n">
-        <v>41.98674281714515</v>
-      </c>
-      <c r="K49" t="n">
-        <v>48.27828996392513</v>
-      </c>
-      <c r="L49" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -2344,33 +1973,26 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>109.0173667560747</v>
+        <v>450</v>
       </c>
       <c r="D50" t="n">
-        <v>15830392</v>
+        <v>359280883.8736283</v>
       </c>
       <c r="E50" t="n">
-        <v>1089581272.101412</v>
+        <v>0.004117087719275794</v>
       </c>
       <c r="F50" t="n">
-        <v>0.003420734654828393</v>
-      </c>
-      <c r="G50" t="n">
-        <v>7.919499420304849</v>
+        <v>0.007290646726758029</v>
+      </c>
+      <c r="G50" t="b">
+        <v>0</v>
       </c>
       <c r="H50" t="n">
-        <v>50000</v>
+        <v>9.113308408447537e-05</v>
       </c>
       <c r="I50" t="n">
-        <v>62192.40520644223</v>
-      </c>
-      <c r="J50" t="n">
-        <v>31.90408850427394</v>
-      </c>
-      <c r="K50" t="n">
-        <v>39.82358792457879</v>
-      </c>
-      <c r="L50" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -2382,33 +2004,26 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>190.2967582920965</v>
+        <v>450</v>
       </c>
       <c r="D51" t="n">
-        <v>15951736</v>
+        <v>4219535299.831759</v>
       </c>
       <c r="E51" t="n">
-        <v>1622337169.092064</v>
+        <v>0.003828359196453526</v>
       </c>
       <c r="F51" t="n">
-        <v>0.004705874959087097</v>
-      </c>
-      <c r="G51" t="n">
-        <v>9.355526421274616</v>
+        <v>0.0006207768898400826</v>
+      </c>
+      <c r="G51" t="b">
+        <v>0</v>
       </c>
       <c r="H51" t="n">
-        <v>50000</v>
+        <v>7.759711123001032e-06</v>
       </c>
       <c r="I51" t="n">
-        <v>76362.27612675549</v>
-      </c>
-      <c r="J51" t="n">
-        <v>25.98392950868037</v>
-      </c>
-      <c r="K51" t="n">
-        <v>35.33945592995498</v>
-      </c>
-      <c r="L51" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -2420,33 +2035,26 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>193.7928751952413</v>
+        <v>450</v>
       </c>
       <c r="D52" t="n">
-        <v>15797112</v>
+        <v>954254552.2521319</v>
       </c>
       <c r="E52" t="n">
-        <v>708604098.0621765</v>
+        <v>0.001412328568693233</v>
       </c>
       <c r="F52" t="n">
-        <v>0.004463609648103219</v>
-      </c>
-      <c r="G52" t="n">
-        <v>21.60139747027422</v>
+        <v>0.002744959396649447</v>
+      </c>
+      <c r="G52" t="b">
+        <v>0</v>
       </c>
       <c r="H52" t="n">
-        <v>50000</v>
+        <v>3.431199245811809e-05</v>
       </c>
       <c r="I52" t="n">
-        <v>73895.36193488157</v>
-      </c>
-      <c r="J52" t="n">
-        <v>26.85137399757943</v>
-      </c>
-      <c r="K52" t="n">
-        <v>48.45277146785365</v>
-      </c>
-      <c r="L52" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -2458,33 +2066,26 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>183.2754091322404</v>
+        <v>450</v>
       </c>
       <c r="D53" t="n">
-        <v>16012152</v>
+        <v>2291055280.461979</v>
       </c>
       <c r="E53" t="n">
-        <v>534924099.7462332</v>
+        <v>0.004736402605423769</v>
       </c>
       <c r="F53" t="n">
-        <v>0.002366384885061197</v>
-      </c>
-      <c r="G53" t="n">
-        <v>27.43037479784332</v>
+        <v>0.001143311565782827</v>
+      </c>
+      <c r="G53" t="b">
+        <v>0</v>
       </c>
       <c r="H53" t="n">
-        <v>50000</v>
+        <v>1.429139457228534e-05</v>
       </c>
       <c r="I53" t="n">
-        <v>48046.11667234816</v>
-      </c>
-      <c r="J53" t="n">
-        <v>41.29765603183402</v>
-      </c>
-      <c r="K53" t="n">
-        <v>68.72803082967735</v>
-      </c>
-      <c r="L53" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -2496,33 +2097,26 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>124.7895474243269</v>
+        <v>450</v>
       </c>
       <c r="D54" t="n">
-        <v>15789944</v>
+        <v>3365275118.556035</v>
       </c>
       <c r="E54" t="n">
-        <v>972513411.8786099</v>
+        <v>0.001346257052656834</v>
       </c>
       <c r="F54" t="n">
-        <v>0.001990437321046356</v>
-      </c>
-      <c r="G54" t="n">
-        <v>10.13055419878063</v>
+        <v>0.0007783583533948697</v>
+      </c>
+      <c r="G54" t="b">
+        <v>0</v>
       </c>
       <c r="H54" t="n">
-        <v>50000</v>
+        <v>9.729479417435871e-06</v>
       </c>
       <c r="I54" t="n">
-        <v>42246.39300708604</v>
-      </c>
-      <c r="J54" t="n">
-        <v>46.96713396732329</v>
-      </c>
-      <c r="K54" t="n">
-        <v>57.09768816610392</v>
-      </c>
-      <c r="L54" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -2534,33 +2128,26 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>176.9190815397503</v>
+        <v>450</v>
       </c>
       <c r="D55" t="n">
-        <v>16121720</v>
+        <v>3439468185.650774</v>
       </c>
       <c r="E55" t="n">
-        <v>496626724.993165</v>
+        <v>0.00430650422421788</v>
       </c>
       <c r="F55" t="n">
-        <v>0.002586423707422875</v>
-      </c>
-      <c r="G55" t="n">
-        <v>28.71613378519126</v>
+        <v>0.0007615683177207207</v>
+      </c>
+      <c r="G55" t="b">
+        <v>0</v>
       </c>
       <c r="H55" t="n">
-        <v>50000</v>
+        <v>9.519603971509009e-06</v>
       </c>
       <c r="I55" t="n">
-        <v>51236.1775502763</v>
-      </c>
-      <c r="J55" t="n">
-        <v>38.72638621515004</v>
-      </c>
-      <c r="K55" t="n">
-        <v>67.44252000034129</v>
-      </c>
-      <c r="L55" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
@@ -2572,33 +2159,26 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>193.9882784309975</v>
+        <v>450</v>
       </c>
       <c r="D56" t="n">
-        <v>15985528</v>
+        <v>3345305167.650477</v>
       </c>
       <c r="E56" t="n">
-        <v>399621228.3434077</v>
+        <v>0.002130840779414419</v>
       </c>
       <c r="F56" t="n">
-        <v>0.001484277804509112</v>
-      </c>
-      <c r="G56" t="n">
-        <v>38.79930339768776</v>
+        <v>0.0007830047988834715</v>
+      </c>
+      <c r="G56" t="b">
+        <v>0</v>
       </c>
       <c r="H56" t="n">
-        <v>50000</v>
+        <v>9.787559986043394e-06</v>
       </c>
       <c r="I56" t="n">
-        <v>33619.50741025421</v>
-      </c>
-      <c r="J56" t="n">
-        <v>59.01906817929182</v>
-      </c>
-      <c r="K56" t="n">
-        <v>97.81837157697959</v>
-      </c>
-      <c r="L56" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -2610,33 +2190,26 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>80.99498629111319</v>
+        <v>450</v>
       </c>
       <c r="D57" t="n">
-        <v>16487288</v>
+        <v>2596785918.423921</v>
       </c>
       <c r="E57" t="n">
-        <v>360598284.0251551</v>
+        <v>0.004455317385926043</v>
       </c>
       <c r="F57" t="n">
-        <v>0.001618486085299413</v>
-      </c>
-      <c r="G57" t="n">
-        <v>18.51627870537065</v>
+        <v>0.001008704638074208</v>
+      </c>
+      <c r="G57" t="b">
+        <v>0</v>
       </c>
       <c r="H57" t="n">
-        <v>50000</v>
+        <v>1.26088079759276e-05</v>
       </c>
       <c r="I57" t="n">
-        <v>36009.3009778573</v>
-      </c>
-      <c r="J57" t="n">
-        <v>55.10220821059848</v>
-      </c>
-      <c r="K57" t="n">
-        <v>73.61848691596913</v>
-      </c>
-      <c r="L57" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -2648,33 +2221,26 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>196.9778996561049</v>
+        <v>450</v>
       </c>
       <c r="D58" t="n">
-        <v>16185208</v>
+        <v>1716606899.486934</v>
       </c>
       <c r="E58" t="n">
-        <v>1323468717.957133</v>
+        <v>0.003302790666920774</v>
       </c>
       <c r="F58" t="n">
-        <v>0.004067192738554019</v>
-      </c>
-      <c r="G58" t="n">
-        <v>12.04459249425361</v>
+        <v>0.001525911378302681</v>
+      </c>
+      <c r="G58" t="b">
+        <v>0</v>
       </c>
       <c r="H58" t="n">
-        <v>50000</v>
+        <v>1.907389222878352e-05</v>
       </c>
       <c r="I58" t="n">
-        <v>69667.43510972674</v>
-      </c>
-      <c r="J58" t="n">
-        <v>28.48091072787282</v>
-      </c>
-      <c r="K58" t="n">
-        <v>40.52550322212643</v>
-      </c>
-      <c r="L58" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -2686,34 +2252,25 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>133.1850064410978</v>
+        <v>450</v>
       </c>
       <c r="D59" t="n">
-        <v>15837560</v>
+        <v>742572680.1132398</v>
       </c>
       <c r="E59" t="n">
-        <v>685074362.7083012</v>
+        <v>0.004950081361062611</v>
       </c>
       <c r="F59" t="n">
-        <v>0.003605196366065674</v>
-      </c>
-      <c r="G59" t="n">
-        <v>15.3948654732348</v>
+        <v>0.00352745269271225</v>
+      </c>
+      <c r="G59" t="b">
+        <v>0</v>
       </c>
       <c r="H59" t="n">
-        <v>50000</v>
+        <v>4.409315865890313e-05</v>
       </c>
       <c r="I59" t="n">
-        <v>64405.48017837193</v>
-      </c>
-      <c r="J59" t="n">
-        <v>30.80781316286674</v>
-      </c>
-      <c r="K59" t="n">
-        <v>46.20267863610155</v>
-      </c>
-      <c r="L59" t="b">
-        <v>1</v>
+        <v>450</v>
       </c>
     </row>
     <row r="60">
@@ -2726,33 +2283,26 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>70.04451452417976</v>
+        <v>450</v>
       </c>
       <c r="D60" t="n">
-        <v>15721848</v>
+        <v>136991014.4672385</v>
       </c>
       <c r="E60" t="n">
-        <v>1469413533.552498</v>
+        <v>0.002288326169720766</v>
       </c>
       <c r="F60" t="n">
-        <v>0.002199761760403742</v>
-      </c>
-      <c r="G60" t="n">
-        <v>3.747172546861542</v>
+        <v>0.01912088913412952</v>
+      </c>
+      <c r="G60" t="b">
+        <v>0</v>
       </c>
       <c r="H60" t="n">
-        <v>50000</v>
+        <v>0.000239011114176619</v>
       </c>
       <c r="I60" t="n">
-        <v>45532.97654412978</v>
-      </c>
-      <c r="J60" t="n">
-        <v>43.57703252887399</v>
-      </c>
-      <c r="K60" t="n">
-        <v>47.32420507573553</v>
-      </c>
-      <c r="L60" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
@@ -2764,33 +2314,26 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>142.0586759530583</v>
+        <v>450</v>
       </c>
       <c r="D61" t="n">
-        <v>16048504</v>
+        <v>4979676526.003522</v>
       </c>
       <c r="E61" t="n">
-        <v>1649671076.535328</v>
+        <v>0.004742895865197575</v>
       </c>
       <c r="F61" t="n">
-        <v>0.00311157923994595</v>
-      </c>
-      <c r="G61" t="n">
-        <v>6.909950903835639</v>
+        <v>0.0005260160948852258</v>
+      </c>
+      <c r="G61" t="b">
+        <v>0</v>
       </c>
       <c r="H61" t="n">
-        <v>50000</v>
+        <v>6.575201186065322e-06</v>
       </c>
       <c r="I61" t="n">
-        <v>58323.93719318287</v>
-      </c>
-      <c r="J61" t="n">
-        <v>34.02019986112872</v>
-      </c>
-      <c r="K61" t="n">
-        <v>40.93015076496435</v>
-      </c>
-      <c r="L61" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
@@ -2802,33 +2345,26 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>185.0524102567513</v>
+        <v>450</v>
       </c>
       <c r="D62" t="n">
-        <v>16051064</v>
+        <v>1054909517.324069</v>
       </c>
       <c r="E62" t="n">
-        <v>788613841.6590987</v>
+        <v>0.003188844578732259</v>
       </c>
       <c r="F62" t="n">
-        <v>0.001822735311748371</v>
-      </c>
-      <c r="G62" t="n">
-        <v>18.8323354440269</v>
+        <v>0.002483047083170188</v>
+      </c>
+      <c r="G62" t="b">
+        <v>0</v>
       </c>
       <c r="H62" t="n">
-        <v>50000</v>
+        <v>3.103808853962735e-05</v>
       </c>
       <c r="I62" t="n">
-        <v>39500.82027205481</v>
-      </c>
-      <c r="J62" t="n">
-        <v>50.23166573084391</v>
-      </c>
-      <c r="K62" t="n">
-        <v>69.06400117487081</v>
-      </c>
-      <c r="L62" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -2840,33 +2376,26 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>78.48125280562525</v>
+        <v>450</v>
       </c>
       <c r="D63" t="n">
-        <v>16320888</v>
+        <v>2775505419.79611</v>
       </c>
       <c r="E63" t="n">
-        <v>1237549364.949501</v>
+        <v>0.00336570255081632</v>
       </c>
       <c r="F63" t="n">
-        <v>0.002997499863290644</v>
-      </c>
-      <c r="G63" t="n">
-        <v>5.175081388339459</v>
+        <v>0.0009437524356167253</v>
+      </c>
+      <c r="G63" t="b">
+        <v>0</v>
       </c>
       <c r="H63" t="n">
-        <v>50000</v>
+        <v>1.179690544520907e-05</v>
       </c>
       <c r="I63" t="n">
-        <v>56842.37841582947</v>
-      </c>
-      <c r="J63" t="n">
-        <v>34.9069137375758</v>
-      </c>
-      <c r="K63" t="n">
-        <v>40.08199512591526</v>
-      </c>
-      <c r="L63" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -2878,33 +2407,26 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>55.88863915004581</v>
+        <v>450</v>
       </c>
       <c r="D64" t="n">
-        <v>15796088</v>
+        <v>2396206003.306677</v>
       </c>
       <c r="E64" t="n">
-        <v>1359397718.505018</v>
+        <v>0.00331276669887613</v>
       </c>
       <c r="F64" t="n">
-        <v>0.004138414173477148</v>
-      </c>
-      <c r="G64" t="n">
-        <v>3.247106605362124</v>
+        <v>0.001093140571547412</v>
+      </c>
+      <c r="G64" t="b">
+        <v>0</v>
       </c>
       <c r="H64" t="n">
-        <v>50000</v>
+        <v>1.366425714434265e-05</v>
       </c>
       <c r="I64" t="n">
-        <v>70445.52738463182</v>
-      </c>
-      <c r="J64" t="n">
-        <v>28.16633040684518</v>
-      </c>
-      <c r="K64" t="n">
-        <v>31.4134370122073</v>
-      </c>
-      <c r="L64" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -2916,33 +2438,26 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>76.25777611248036</v>
+        <v>450</v>
       </c>
       <c r="D65" t="n">
-        <v>16320888</v>
+        <v>1820272257.570522</v>
       </c>
       <c r="E65" t="n">
-        <v>822043245.1002465</v>
+        <v>0.003427462180662559</v>
       </c>
       <c r="F65" t="n">
-        <v>0.003270637843220156</v>
-      </c>
-      <c r="G65" t="n">
-        <v>7.570128642740027</v>
+        <v>0.001439010010236624</v>
+      </c>
+      <c r="G65" t="b">
+        <v>0</v>
       </c>
       <c r="H65" t="n">
-        <v>50000</v>
+        <v>1.79876251279578e-05</v>
       </c>
       <c r="I65" t="n">
-        <v>60340.13487674308</v>
-      </c>
-      <c r="J65" t="n">
-        <v>32.88345317843775</v>
-      </c>
-      <c r="K65" t="n">
-        <v>40.45358182117778</v>
-      </c>
-      <c r="L65" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -2954,33 +2469,26 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>86.26424141379189</v>
+        <v>450</v>
       </c>
       <c r="D66" t="n">
-        <v>15873400</v>
+        <v>3590032980.804874</v>
       </c>
       <c r="E66" t="n">
-        <v>738439476.8861331</v>
+        <v>0.00443694832660471</v>
       </c>
       <c r="F66" t="n">
-        <v>0.003396614112301707</v>
-      </c>
-      <c r="G66" t="n">
-        <v>9.271625180656685</v>
+        <v>0.0007296283945037019</v>
+      </c>
+      <c r="G66" t="b">
+        <v>0</v>
       </c>
       <c r="H66" t="n">
-        <v>50000</v>
+        <v>9.120354931296274e-06</v>
       </c>
       <c r="I66" t="n">
-        <v>61897.93445756329</v>
-      </c>
-      <c r="J66" t="n">
-        <v>32.055867734332</v>
-      </c>
-      <c r="K66" t="n">
-        <v>41.32749291498869</v>
-      </c>
-      <c r="L66" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
@@ -2992,33 +2500,26 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>111.4556148150323</v>
+        <v>450</v>
       </c>
       <c r="D67" t="n">
-        <v>16164728</v>
+        <v>1500136043.622596</v>
       </c>
       <c r="E67" t="n">
-        <v>1996537153.621115</v>
+        <v>0.001518861118453455</v>
       </c>
       <c r="F67" t="n">
-        <v>0.003285507832309029</v>
-      </c>
-      <c r="G67" t="n">
-        <v>4.511936315059602</v>
+        <v>0.001746101636005345</v>
+      </c>
+      <c r="G67" t="b">
+        <v>0</v>
       </c>
       <c r="H67" t="n">
-        <v>50000</v>
+        <v>2.182627045006682e-05</v>
       </c>
       <c r="I67" t="n">
-        <v>60525.77524472695</v>
-      </c>
-      <c r="J67" t="n">
-        <v>32.78259538150838</v>
-      </c>
-      <c r="K67" t="n">
-        <v>37.29453169656798</v>
-      </c>
-      <c r="L67" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
@@ -3030,33 +2531,26 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>71.46350257963377</v>
+        <v>450</v>
       </c>
       <c r="D68" t="n">
-        <v>15692152</v>
+        <v>4145381257.923578</v>
       </c>
       <c r="E68" t="n">
-        <v>901279984.4324811</v>
+        <v>0.003089037554167409</v>
       </c>
       <c r="F68" t="n">
-        <v>0.002129916837931281</v>
-      </c>
-      <c r="G68" t="n">
-        <v>6.221241813320306</v>
+        <v>0.0006318815657771495</v>
+      </c>
+      <c r="G68" t="b">
+        <v>0</v>
       </c>
       <c r="H68" t="n">
-        <v>50000</v>
+        <v>7.898519572214369e-06</v>
       </c>
       <c r="I68" t="n">
-        <v>44452.909264879</v>
-      </c>
-      <c r="J68" t="n">
-        <v>44.63581873071364</v>
-      </c>
-      <c r="K68" t="n">
-        <v>50.85706054403395</v>
-      </c>
-      <c r="L68" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
@@ -3068,33 +2562,26 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>131.0427524504756</v>
+        <v>450</v>
       </c>
       <c r="D69" t="n">
-        <v>16206712</v>
+        <v>3516472082.361291</v>
       </c>
       <c r="E69" t="n">
-        <v>1180510491.86085</v>
+        <v>0.002974308754870507</v>
       </c>
       <c r="F69" t="n">
-        <v>0.00263717341161561</v>
-      </c>
-      <c r="G69" t="n">
-        <v>8.995143047413451</v>
+        <v>0.0007448914533230404</v>
+      </c>
+      <c r="G69" t="b">
+        <v>0</v>
       </c>
       <c r="H69" t="n">
-        <v>50000</v>
+        <v>9.311143166538005e-06</v>
       </c>
       <c r="I69" t="n">
-        <v>51952.33397837322</v>
-      </c>
-      <c r="J69" t="n">
-        <v>38.19254782327935</v>
-      </c>
-      <c r="K69" t="n">
-        <v>47.1876908706928</v>
-      </c>
-      <c r="L69" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
@@ -3106,34 +2593,25 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>54.93064420429195</v>
+        <v>450</v>
       </c>
       <c r="D70" t="n">
-        <v>15398264</v>
+        <v>4332103328.278568</v>
       </c>
       <c r="E70" t="n">
-        <v>774775253.9326193</v>
+        <v>0.001063109582620098</v>
       </c>
       <c r="F70" t="n">
-        <v>0.003163815307212136</v>
-      </c>
-      <c r="G70" t="n">
-        <v>5.458593036202717</v>
+        <v>0.0006046462426003254</v>
+      </c>
+      <c r="G70" t="b">
+        <v>0</v>
       </c>
       <c r="H70" t="n">
-        <v>50000</v>
+        <v>7.558078032504067e-06</v>
       </c>
       <c r="I70" t="n">
-        <v>58992.30630462984</v>
-      </c>
-      <c r="J70" t="n">
-        <v>33.63475890828626</v>
-      </c>
-      <c r="K70" t="n">
-        <v>39.09335194448897</v>
-      </c>
-      <c r="L70" t="b">
-        <v>1</v>
+        <v>450</v>
       </c>
     </row>
     <row r="71">
@@ -3146,33 +2624,26 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>176.856958673085</v>
+        <v>450</v>
       </c>
       <c r="D71" t="n">
-        <v>15725432</v>
+        <v>504297073.4791481</v>
       </c>
       <c r="E71" t="n">
-        <v>1446158044.094196</v>
+        <v>0.004812645225515649</v>
       </c>
       <c r="F71" t="n">
-        <v>0.004652738496630695</v>
-      </c>
-      <c r="G71" t="n">
-        <v>9.615657461153875</v>
+        <v>0.00519414079072245</v>
+      </c>
+      <c r="G71" t="b">
+        <v>0</v>
       </c>
       <c r="H71" t="n">
-        <v>50000</v>
+        <v>6.492675988403063e-05</v>
       </c>
       <c r="I71" t="n">
-        <v>75828.38014114599</v>
-      </c>
-      <c r="J71" t="n">
-        <v>26.16687836805495</v>
-      </c>
-      <c r="K71" t="n">
-        <v>35.78253582920882</v>
-      </c>
-      <c r="L71" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
@@ -3184,33 +2655,26 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>69.68289341912946</v>
+        <v>450</v>
       </c>
       <c r="D72" t="n">
-        <v>15849336</v>
+        <v>4630688955.057376</v>
       </c>
       <c r="E72" t="n">
-        <v>1954913180.385197</v>
+        <v>0.002809482020246182</v>
       </c>
       <c r="F72" t="n">
-        <v>0.002940043533152437</v>
-      </c>
-      <c r="G72" t="n">
-        <v>2.824748439811416</v>
+        <v>0.0005656588091798415</v>
+      </c>
+      <c r="G72" t="b">
+        <v>0</v>
       </c>
       <c r="H72" t="n">
-        <v>50000</v>
+        <v>7.070735114748019e-06</v>
       </c>
       <c r="I72" t="n">
-        <v>56084.50507952144</v>
-      </c>
-      <c r="J72" t="n">
-        <v>35.3786129909971</v>
-      </c>
-      <c r="K72" t="n">
-        <v>38.20336143080851</v>
-      </c>
-      <c r="L72" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
@@ -3222,33 +2686,26 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>174.4587486684707</v>
+        <v>450</v>
       </c>
       <c r="D73" t="n">
-        <v>16135544</v>
+        <v>2660087432.532396</v>
       </c>
       <c r="E73" t="n">
-        <v>1983211705.301169</v>
+        <v>0.002224968725751194</v>
       </c>
       <c r="F73" t="n">
-        <v>0.004141769499025968</v>
-      </c>
-      <c r="G73" t="n">
-        <v>7.097040643216576</v>
+        <v>0.0009847007162115523</v>
+      </c>
+      <c r="G73" t="b">
+        <v>0</v>
       </c>
       <c r="H73" t="n">
-        <v>50000</v>
+        <v>1.23087589526444e-05</v>
       </c>
       <c r="I73" t="n">
-        <v>70481.97802230541</v>
-      </c>
-      <c r="J73" t="n">
-        <v>28.15176383631094</v>
-      </c>
-      <c r="K73" t="n">
-        <v>35.24880447952751</v>
-      </c>
-      <c r="L73" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
@@ -3260,34 +2717,25 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>82.55233018306427</v>
+        <v>450</v>
       </c>
       <c r="D74" t="n">
-        <v>15966584</v>
+        <v>1464896044.314089</v>
       </c>
       <c r="E74" t="n">
-        <v>1703996531.976969</v>
+        <v>0.003468514637626379</v>
       </c>
       <c r="F74" t="n">
-        <v>0.0007562525827702932</v>
-      </c>
-      <c r="G74" t="n">
-        <v>3.867609732557383</v>
+        <v>0.001788106405343241</v>
+      </c>
+      <c r="G74" t="b">
+        <v>0</v>
       </c>
       <c r="H74" t="n">
-        <v>50000</v>
+        <v>2.235133006679052e-05</v>
       </c>
       <c r="I74" t="n">
-        <v>19064.22584051994</v>
-      </c>
-      <c r="J74" t="n">
-        <v>104.079337739627</v>
-      </c>
-      <c r="K74" t="n">
-        <v>107.9469474721844</v>
-      </c>
-      <c r="L74" t="b">
-        <v>1</v>
+        <v>450</v>
       </c>
     </row>
     <row r="75">
@@ -3300,33 +2748,26 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>184.2077631581811</v>
+        <v>450</v>
       </c>
       <c r="D75" t="n">
-        <v>15621496</v>
+        <v>1176742228.621739</v>
       </c>
       <c r="E75" t="n">
-        <v>1668267201.057022</v>
+        <v>0.000635704185960415</v>
       </c>
       <c r="F75" t="n">
-        <v>0.002482675921991459</v>
-      </c>
-      <c r="G75" t="n">
-        <v>8.6245202013239</v>
+        <v>0.002225967536720395</v>
+      </c>
+      <c r="G75" t="b">
+        <v>0</v>
       </c>
       <c r="H75" t="n">
-        <v>50000</v>
+        <v>2.782459420900493e-05</v>
       </c>
       <c r="I75" t="n">
-        <v>49749.63239599508</v>
-      </c>
-      <c r="J75" t="n">
-        <v>39.88355098197128</v>
-      </c>
-      <c r="K75" t="n">
-        <v>48.50807118329519</v>
-      </c>
-      <c r="L75" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
@@ -3338,33 +2779,26 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>150.4612379226002</v>
+        <v>450</v>
       </c>
       <c r="D76" t="n">
-        <v>15896952</v>
+        <v>4319411996.400764</v>
       </c>
       <c r="E76" t="n">
-        <v>861887180.5557278</v>
+        <v>0.002726813800930032</v>
       </c>
       <c r="F76" t="n">
-        <v>0.003616698532452832</v>
-      </c>
-      <c r="G76" t="n">
-        <v>13.87580144523046</v>
+        <v>0.0006064228191667427</v>
+      </c>
+      <c r="G76" t="b">
+        <v>0</v>
       </c>
       <c r="H76" t="n">
-        <v>50000</v>
+        <v>7.580285239584284e-06</v>
       </c>
       <c r="I76" t="n">
-        <v>64541.2539143033</v>
-      </c>
-      <c r="J76" t="n">
-        <v>30.74300357775159</v>
-      </c>
-      <c r="K76" t="n">
-        <v>44.61880502298204</v>
-      </c>
-      <c r="L76" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
@@ -3376,33 +2810,26 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>87.20671614748089</v>
+        <v>450</v>
       </c>
       <c r="D77" t="n">
-        <v>16294776</v>
+        <v>3601338091.852296</v>
       </c>
       <c r="E77" t="n">
-        <v>351223006.1513095</v>
+        <v>0.00344608582593801</v>
       </c>
       <c r="F77" t="n">
-        <v>0.001038659497402394</v>
-      </c>
-      <c r="G77" t="n">
-        <v>20.22951060197066</v>
+        <v>0.0007273379874902982</v>
+      </c>
+      <c r="G77" t="b">
+        <v>0</v>
       </c>
       <c r="H77" t="n">
-        <v>50000</v>
+        <v>9.091724843628727e-06</v>
       </c>
       <c r="I77" t="n">
-        <v>25063.7426113402</v>
-      </c>
-      <c r="J77" t="n">
-        <v>79.1658305293258</v>
-      </c>
-      <c r="K77" t="n">
-        <v>99.39534113129646</v>
-      </c>
-      <c r="L77" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
@@ -3414,33 +2841,26 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>71.32581947598374</v>
+        <v>450</v>
       </c>
       <c r="D78" t="n">
-        <v>15333240</v>
+        <v>1115656505.398739</v>
       </c>
       <c r="E78" t="n">
-        <v>209264186.4712918</v>
+        <v>0.004005852520261659</v>
       </c>
       <c r="F78" t="n">
-        <v>0.001885223177632071</v>
-      </c>
-      <c r="G78" t="n">
-        <v>26.13098606750773</v>
+        <v>0.002347846301549437</v>
+      </c>
+      <c r="G78" t="b">
+        <v>0</v>
       </c>
       <c r="H78" t="n">
-        <v>50000</v>
+        <v>2.934807876936797e-05</v>
       </c>
       <c r="I78" t="n">
-        <v>40536.10864420272</v>
-      </c>
-      <c r="J78" t="n">
-        <v>48.94875374979463</v>
-      </c>
-      <c r="K78" t="n">
-        <v>75.07973981730235</v>
-      </c>
-      <c r="L78" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
@@ -3452,33 +2872,26 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>74.28021156810651</v>
+        <v>450</v>
       </c>
       <c r="D79" t="n">
-        <v>15767416</v>
+        <v>2736362818.375944</v>
       </c>
       <c r="E79" t="n">
-        <v>1534460904.04586</v>
+        <v>0.001681140985233018</v>
       </c>
       <c r="F79" t="n">
-        <v>0.001666109683140862</v>
-      </c>
-      <c r="G79" t="n">
-        <v>3.816346813640761</v>
+        <v>0.0009572524456221897</v>
+      </c>
+      <c r="G79" t="b">
+        <v>0</v>
       </c>
       <c r="H79" t="n">
-        <v>50000</v>
+        <v>1.196565557027737e-05</v>
       </c>
       <c r="I79" t="n">
-        <v>36838.63637530821</v>
-      </c>
-      <c r="J79" t="n">
-        <v>53.86171137783867</v>
-      </c>
-      <c r="K79" t="n">
-        <v>57.67805819147944</v>
-      </c>
-      <c r="L79" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
@@ -3490,34 +2903,25 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>179.1929665317418</v>
+        <v>450</v>
       </c>
       <c r="D80" t="n">
-        <v>16004472</v>
+        <v>3802107466.613652</v>
       </c>
       <c r="E80" t="n">
-        <v>560377062.412035</v>
+        <v>0.004946010538108961</v>
       </c>
       <c r="F80" t="n">
-        <v>0.00193089194107558</v>
-      </c>
-      <c r="G80" t="n">
-        <v>25.58892045928793</v>
+        <v>0.0006889310791451564</v>
+      </c>
+      <c r="G80" t="b">
+        <v>0</v>
       </c>
       <c r="H80" t="n">
-        <v>50000</v>
+        <v>8.611638489314455e-06</v>
       </c>
       <c r="I80" t="n">
-        <v>41283.45242310174</v>
-      </c>
-      <c r="J80" t="n">
-        <v>48.06264698176427</v>
-      </c>
-      <c r="K80" t="n">
-        <v>73.65156744105221</v>
-      </c>
-      <c r="L80" t="b">
-        <v>1</v>
+        <v>450</v>
       </c>
     </row>
     <row r="81">
@@ -3530,33 +2934,26 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>72.12315888514658</v>
+        <v>450</v>
       </c>
       <c r="D81" t="n">
-        <v>16419192</v>
+        <v>4206508177.990417</v>
       </c>
       <c r="E81" t="n">
-        <v>1321342249.073822</v>
+        <v>0.004994294820225974</v>
       </c>
       <c r="F81" t="n">
-        <v>0.00448652081697639</v>
-      </c>
-      <c r="G81" t="n">
-        <v>4.481064592507281</v>
+        <v>0.0006226993718222998</v>
+      </c>
+      <c r="G81" t="b">
+        <v>0</v>
       </c>
       <c r="H81" t="n">
-        <v>50000</v>
+        <v>7.783742147778748e-06</v>
       </c>
       <c r="I81" t="n">
-        <v>74132.30494782596</v>
-      </c>
-      <c r="J81" t="n">
-        <v>26.7655511506956</v>
-      </c>
-      <c r="K81" t="n">
-        <v>31.24661574320288</v>
-      </c>
-      <c r="L81" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
@@ -3568,34 +2965,25 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>172.8535067844344</v>
+        <v>450</v>
       </c>
       <c r="D82" t="n">
-        <v>16084856</v>
+        <v>1499691726.662421</v>
       </c>
       <c r="E82" t="n">
-        <v>1022957066.133567</v>
+        <v>0.0007745767983105118</v>
       </c>
       <c r="F82" t="n">
-        <v>0.001606508508977241</v>
-      </c>
-      <c r="G82" t="n">
-        <v>13.58964055173565</v>
+        <v>0.001746618957370311</v>
+      </c>
+      <c r="G82" t="b">
+        <v>0</v>
       </c>
       <c r="H82" t="n">
-        <v>50000</v>
+        <v>2.183273696712889e-05</v>
       </c>
       <c r="I82" t="n">
-        <v>35799.20962790337</v>
-      </c>
-      <c r="J82" t="n">
-        <v>55.4255811964474</v>
-      </c>
-      <c r="K82" t="n">
-        <v>69.01522174818305</v>
-      </c>
-      <c r="L82" t="b">
-        <v>1</v>
+        <v>450</v>
       </c>
     </row>
     <row r="83">
@@ -3608,33 +2996,26 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>171.6807712561013</v>
+        <v>450</v>
       </c>
       <c r="D83" t="n">
-        <v>15918456</v>
+        <v>870360888.1690898</v>
       </c>
       <c r="E83" t="n">
-        <v>1210767302.302867</v>
+        <v>0.003172261218609759</v>
       </c>
       <c r="F83" t="n">
-        <v>0.0009795826408700182</v>
-      </c>
-      <c r="G83" t="n">
-        <v>11.28578876423397</v>
+        <v>0.003009544702209915</v>
+      </c>
+      <c r="G83" t="b">
+        <v>0</v>
       </c>
       <c r="H83" t="n">
-        <v>50000</v>
+        <v>3.761930877762393e-05</v>
       </c>
       <c r="I83" t="n">
-        <v>23849.30886311855</v>
-      </c>
-      <c r="J83" t="n">
-        <v>83.19704404803224</v>
-      </c>
-      <c r="K83" t="n">
-        <v>94.48283281226621</v>
-      </c>
-      <c r="L83" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
@@ -3646,33 +3027,26 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>123.6215965024742</v>
+        <v>450</v>
       </c>
       <c r="D84" t="n">
-        <v>16279928</v>
+        <v>2323146945.48481</v>
       </c>
       <c r="E84" t="n">
-        <v>417404864.1657931</v>
+        <v>0.002935398776652351</v>
       </c>
       <c r="F84" t="n">
-        <v>0.004889361258822273</v>
-      </c>
-      <c r="G84" t="n">
-        <v>24.10789694949442</v>
+        <v>0.001127518000999015</v>
+      </c>
+      <c r="G84" t="b">
+        <v>0</v>
       </c>
       <c r="H84" t="n">
-        <v>50000</v>
+        <v>1.409397501248768e-05</v>
       </c>
       <c r="I84" t="n">
-        <v>78176.07836895097</v>
-      </c>
-      <c r="J84" t="n">
-        <v>25.38106338150696</v>
-      </c>
-      <c r="K84" t="n">
-        <v>49.48896033100138</v>
-      </c>
-      <c r="L84" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
@@ -3684,33 +3058,26 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>154.3020897871861</v>
+        <v>450</v>
       </c>
       <c r="D85" t="n">
-        <v>16257912</v>
+        <v>3711973462.863582</v>
       </c>
       <c r="E85" t="n">
-        <v>1322438604.389314</v>
+        <v>0.001731753187169573</v>
       </c>
       <c r="F85" t="n">
-        <v>0.003245631766860942</v>
-      </c>
-      <c r="G85" t="n">
-        <v>9.484862997986301</v>
+        <v>0.0007056596783909349</v>
+      </c>
+      <c r="G85" t="b">
+        <v>0</v>
       </c>
       <c r="H85" t="n">
-        <v>50000</v>
+        <v>8.820745979886685e-06</v>
       </c>
       <c r="I85" t="n">
-        <v>60026.87198628486</v>
-      </c>
-      <c r="J85" t="n">
-        <v>33.05506241360294</v>
-      </c>
-      <c r="K85" t="n">
-        <v>42.53992541158924</v>
-      </c>
-      <c r="L85" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
@@ -3722,33 +3089,26 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>107.2893048622893</v>
+        <v>450</v>
       </c>
       <c r="D86" t="n">
-        <v>15758200</v>
+        <v>1853577278.109043</v>
       </c>
       <c r="E86" t="n">
-        <v>1455196244.606745</v>
+        <v>0.003016779688830322</v>
       </c>
       <c r="F86" t="n">
-        <v>0.0006961134820553428</v>
-      </c>
-      <c r="G86" t="n">
-        <v>5.809135125750069</v>
+        <v>0.001413153921843611</v>
+      </c>
+      <c r="G86" t="b">
+        <v>0</v>
       </c>
       <c r="H86" t="n">
-        <v>50000</v>
+        <v>1.766442402304514e-05</v>
       </c>
       <c r="I86" t="n">
-        <v>17719.52695008869</v>
-      </c>
-      <c r="J86" t="n">
-        <v>111.9777071695511</v>
-      </c>
-      <c r="K86" t="n">
-        <v>117.7868422953012</v>
-      </c>
-      <c r="L86" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
@@ -3760,33 +3120,26 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>106.4737197173159</v>
+        <v>450</v>
       </c>
       <c r="D87" t="n">
-        <v>15856504</v>
+        <v>1389707911.595429</v>
       </c>
       <c r="E87" t="n">
-        <v>1134281407.324714</v>
+        <v>0.003072457253250685</v>
       </c>
       <c r="F87" t="n">
-        <v>0.0008366285255963879</v>
-      </c>
-      <c r="G87" t="n">
-        <v>7.442160965039881</v>
+        <v>0.001884849311243293</v>
+      </c>
+      <c r="G87" t="b">
+        <v>0</v>
       </c>
       <c r="H87" t="n">
-        <v>50000</v>
+        <v>2.356061639054116e-05</v>
       </c>
       <c r="I87" t="n">
-        <v>20823.14910349498</v>
-      </c>
-      <c r="J87" t="n">
-        <v>95.28779677551131</v>
-      </c>
-      <c r="K87" t="n">
-        <v>102.7299577405512</v>
-      </c>
-      <c r="L87" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
@@ -3798,34 +3151,25 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>53.45133968940532</v>
+        <v>450</v>
       </c>
       <c r="D88" t="n">
-        <v>16629112</v>
+        <v>2923311899.978363</v>
       </c>
       <c r="E88" t="n">
-        <v>650238407.3713324</v>
+        <v>0.0009117920891983977</v>
       </c>
       <c r="F88" t="n">
-        <v>0.0007065356584511728</v>
-      </c>
-      <c r="G88" t="n">
-        <v>6.834787857567837</v>
+        <v>0.0008960350758396283</v>
+      </c>
+      <c r="G88" t="b">
+        <v>0</v>
       </c>
       <c r="H88" t="n">
-        <v>50000</v>
+        <v>1.120043844799535e-05</v>
       </c>
       <c r="I88" t="n">
-        <v>17954.36779724315</v>
-      </c>
-      <c r="J88" t="n">
-        <v>110.5130530023267</v>
-      </c>
-      <c r="K88" t="n">
-        <v>117.3478408598945</v>
-      </c>
-      <c r="L88" t="b">
-        <v>1</v>
+        <v>450</v>
       </c>
     </row>
     <row r="89">
@@ -3838,33 +3182,26 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>132.4408171445011</v>
+        <v>450</v>
       </c>
       <c r="D89" t="n">
-        <v>15974264</v>
+        <v>1872636609.152395</v>
       </c>
       <c r="E89" t="n">
-        <v>1158173857.403489</v>
+        <v>0.0005019296093609231</v>
       </c>
       <c r="F89" t="n">
-        <v>0.001350805077311626</v>
-      </c>
-      <c r="G89" t="n">
-        <v>9.133536229979551</v>
+        <v>0.001398771116188744</v>
+      </c>
+      <c r="G89" t="b">
+        <v>0</v>
       </c>
       <c r="H89" t="n">
-        <v>50000</v>
+        <v>1.74846389523593e-05</v>
       </c>
       <c r="I89" t="n">
-        <v>31161.60013851164</v>
-      </c>
-      <c r="J89" t="n">
-        <v>63.67426547996165</v>
-      </c>
-      <c r="K89" t="n">
-        <v>72.8078017099412</v>
-      </c>
-      <c r="L89" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
@@ -3876,33 +3213,26 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>127.8416208440656</v>
+        <v>450</v>
       </c>
       <c r="D90" t="n">
-        <v>16025976</v>
+        <v>483743772.0375717</v>
       </c>
       <c r="E90" t="n">
-        <v>465453896.4985261</v>
+        <v>0.004930920503004112</v>
       </c>
       <c r="F90" t="n">
-        <v>0.001567453460752141</v>
-      </c>
-      <c r="G90" t="n">
-        <v>22.00848207374049</v>
+        <v>0.005414829402282322</v>
+      </c>
+      <c r="G90" t="b">
+        <v>0</v>
       </c>
       <c r="H90" t="n">
-        <v>50000</v>
+        <v>6.768536752852901e-05</v>
       </c>
       <c r="I90" t="n">
-        <v>35109.88719924723</v>
-      </c>
-      <c r="J90" t="n">
-        <v>56.51376743934802</v>
-      </c>
-      <c r="K90" t="n">
-        <v>78.5222495130885</v>
-      </c>
-      <c r="L90" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
@@ -3914,34 +3244,25 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>183.1996448663853</v>
+        <v>450</v>
       </c>
       <c r="D91" t="n">
-        <v>15995768</v>
+        <v>1668980990.983274</v>
       </c>
       <c r="E91" t="n">
-        <v>516511718.664229</v>
+        <v>0.004410033783401334</v>
       </c>
       <c r="F91" t="n">
-        <v>0.0005871966757232473</v>
-      </c>
-      <c r="G91" t="n">
-        <v>28.36740107798098</v>
+        <v>0.00156945466374473</v>
+      </c>
+      <c r="G91" t="b">
+        <v>0</v>
       </c>
       <c r="H91" t="n">
-        <v>50000</v>
+        <v>1.961818329680912e-05</v>
       </c>
       <c r="I91" t="n">
-        <v>15218.46503095147</v>
-      </c>
-      <c r="J91" t="n">
-        <v>130.3805604549822</v>
-      </c>
-      <c r="K91" t="n">
-        <v>158.7479615329632</v>
-      </c>
-      <c r="L91" t="b">
-        <v>1</v>
+        <v>450</v>
       </c>
     </row>
     <row r="92">
@@ -3954,33 +3275,26 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>65.29511316072475</v>
+        <v>450</v>
       </c>
       <c r="D92" t="n">
-        <v>15985016</v>
+        <v>4362899460.142323</v>
       </c>
       <c r="E92" t="n">
-        <v>1194709197.51504</v>
+        <v>0.003740441218364305</v>
       </c>
       <c r="F92" t="n">
-        <v>0.003680621467925245</v>
-      </c>
-      <c r="G92" t="n">
-        <v>4.368190312617293</v>
+        <v>0.0006003782631091281</v>
+      </c>
+      <c r="G92" t="b">
+        <v>0</v>
       </c>
       <c r="H92" t="n">
-        <v>50000</v>
+        <v>7.504728288864101e-06</v>
       </c>
       <c r="I92" t="n">
-        <v>65291.19075123936</v>
-      </c>
-      <c r="J92" t="n">
-        <v>30.38988839336394</v>
-      </c>
-      <c r="K92" t="n">
-        <v>34.75807870598123</v>
-      </c>
-      <c r="L92" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
@@ -3992,33 +3306,26 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>110.0015497956827</v>
+        <v>450</v>
       </c>
       <c r="D93" t="n">
-        <v>16258936</v>
+        <v>467494237.3542276</v>
       </c>
       <c r="E93" t="n">
-        <v>831584283.693337</v>
+        <v>0.003132384002795019</v>
       </c>
       <c r="F93" t="n">
-        <v>0.002061173502285653</v>
-      </c>
-      <c r="G93" t="n">
-        <v>10.7536192848996</v>
+        <v>0.005603042328017506</v>
+      </c>
+      <c r="G93" t="b">
+        <v>0</v>
       </c>
       <c r="H93" t="n">
-        <v>50000</v>
+        <v>7.003802910021883e-05</v>
       </c>
       <c r="I93" t="n">
-        <v>43373.84774838227</v>
-      </c>
-      <c r="J93" t="n">
-        <v>45.74627576300295</v>
-      </c>
-      <c r="K93" t="n">
-        <v>56.49989504790256</v>
-      </c>
-      <c r="L93" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
@@ -4030,33 +3337,26 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>60.91849287194707</v>
+        <v>450</v>
       </c>
       <c r="D94" t="n">
-        <v>15530872</v>
+        <v>3088201717.775626</v>
       </c>
       <c r="E94" t="n">
-        <v>777642540.3487796</v>
+        <v>0.003884378204244046</v>
       </c>
       <c r="F94" t="n">
-        <v>0.0033743617892545</v>
-      </c>
-      <c r="G94" t="n">
-        <v>6.083240474490891</v>
+        <v>0.0008481926504097336</v>
+      </c>
+      <c r="G94" t="b">
+        <v>0</v>
       </c>
       <c r="H94" t="n">
-        <v>50000</v>
+        <v>1.060240813012167e-05</v>
       </c>
       <c r="I94" t="n">
-        <v>61625.20129915526</v>
-      </c>
-      <c r="J94" t="n">
-        <v>32.19773661051227</v>
-      </c>
-      <c r="K94" t="n">
-        <v>38.28097708500317</v>
-      </c>
-      <c r="L94" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
@@ -4068,33 +3368,26 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>111.6800830954083</v>
+        <v>450</v>
       </c>
       <c r="D95" t="n">
-        <v>15910264</v>
+        <v>2864211086.268296</v>
       </c>
       <c r="E95" t="n">
-        <v>147059209.5490601</v>
+        <v>0.0006846881740966699</v>
       </c>
       <c r="F95" t="n">
-        <v>0.001522833470691657</v>
-      </c>
-      <c r="G95" t="n">
-        <v>60.41306800976344</v>
+        <v>0.0009145240769990639</v>
+      </c>
+      <c r="G95" t="b">
+        <v>0</v>
       </c>
       <c r="H95" t="n">
-        <v>50000</v>
+        <v>1.14315509624883e-05</v>
       </c>
       <c r="I95" t="n">
-        <v>34314.19612373249</v>
-      </c>
-      <c r="J95" t="n">
-        <v>57.82423090563638</v>
-      </c>
-      <c r="K95" t="n">
-        <v>118.2372989153998</v>
-      </c>
-      <c r="L95" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
@@ -4106,34 +3399,25 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>147.8631913216177</v>
+        <v>450</v>
       </c>
       <c r="D96" t="n">
-        <v>16429432</v>
+        <v>3929859575.691922</v>
       </c>
       <c r="E96" t="n">
-        <v>1669896637.573479</v>
+        <v>0.003092550209794676</v>
       </c>
       <c r="F96" t="n">
-        <v>0.001417999480976379</v>
-      </c>
-      <c r="G96" t="n">
-        <v>7.273828189304962</v>
+        <v>0.0006665352666039752</v>
+      </c>
+      <c r="G96" t="b">
+        <v>0</v>
       </c>
       <c r="H96" t="n">
-        <v>50000</v>
+        <v>8.33169083254969e-06</v>
       </c>
       <c r="I96" t="n">
-        <v>32409.4555801022</v>
-      </c>
-      <c r="J96" t="n">
-        <v>61.22262668362118</v>
-      </c>
-      <c r="K96" t="n">
-        <v>68.49645487292614</v>
-      </c>
-      <c r="L96" t="b">
-        <v>1</v>
+        <v>450</v>
       </c>
     </row>
     <row r="97">
@@ -4146,34 +3430,25 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>195.7701725952953</v>
+        <v>450</v>
       </c>
       <c r="D97" t="n">
-        <v>16835960</v>
+        <v>356891730.9061045</v>
       </c>
       <c r="E97" t="n">
-        <v>201361257.9122049</v>
+        <v>0.0006378078790579216</v>
       </c>
       <c r="F97" t="n">
-        <v>0.004825213050580189</v>
-      </c>
-      <c r="G97" t="n">
-        <v>81.84242662122627</v>
+        <v>0.007339452761625182</v>
+      </c>
+      <c r="G97" t="b">
+        <v>0</v>
       </c>
       <c r="H97" t="n">
-        <v>50000</v>
+        <v>9.174315952031477e-05</v>
       </c>
       <c r="I97" t="n">
-        <v>77547.13127023033</v>
-      </c>
-      <c r="J97" t="n">
-        <v>25.58691685299923</v>
-      </c>
-      <c r="K97" t="n">
-        <v>107.4293434742255</v>
-      </c>
-      <c r="L97" t="b">
-        <v>1</v>
+        <v>450</v>
       </c>
     </row>
     <row r="98">
@@ -4186,33 +3461,26 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>166.7802708257455</v>
+        <v>450</v>
       </c>
       <c r="D98" t="n">
-        <v>15735672</v>
+        <v>1335580020.245311</v>
       </c>
       <c r="E98" t="n">
-        <v>1407754817.176042</v>
+        <v>0.001147108423694674</v>
       </c>
       <c r="F98" t="n">
-        <v>0.003431813667993422</v>
-      </c>
-      <c r="G98" t="n">
-        <v>9.321224142744009</v>
+        <v>0.001961237784553626</v>
+      </c>
+      <c r="G98" t="b">
+        <v>0</v>
       </c>
       <c r="H98" t="n">
-        <v>50000</v>
+        <v>2.451547230692033e-05</v>
       </c>
       <c r="I98" t="n">
-        <v>62327.25926120698</v>
-      </c>
-      <c r="J98" t="n">
-        <v>31.83505938684806</v>
-      </c>
-      <c r="K98" t="n">
-        <v>41.15628352959207</v>
-      </c>
-      <c r="L98" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
@@ -4224,33 +3492,26 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>61.88632059983418</v>
+        <v>450</v>
       </c>
       <c r="D99" t="n">
-        <v>16168312</v>
+        <v>2976830247.035522</v>
       </c>
       <c r="E99" t="n">
-        <v>125332034.8360715</v>
+        <v>0.003834960458402864</v>
       </c>
       <c r="F99" t="n">
-        <v>0.003593306160108694</v>
-      </c>
-      <c r="G99" t="n">
-        <v>39.91786063710212</v>
+        <v>0.0008799258884877702</v>
+      </c>
+      <c r="G99" t="b">
+        <v>0</v>
       </c>
       <c r="H99" t="n">
-        <v>50000</v>
+        <v>1.099907360609713e-05</v>
       </c>
       <c r="I99" t="n">
-        <v>64264.85679804237</v>
-      </c>
-      <c r="J99" t="n">
-        <v>30.87522635015725</v>
-      </c>
-      <c r="K99" t="n">
-        <v>70.79308698725936</v>
-      </c>
-      <c r="L99" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
@@ -4262,33 +3523,26 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>62.05707620906058</v>
+        <v>450</v>
       </c>
       <c r="D100" t="n">
-        <v>16612728</v>
+        <v>2363047043.720602</v>
       </c>
       <c r="E100" t="n">
-        <v>1374456448.917518</v>
+        <v>0.00169563756115441</v>
       </c>
       <c r="F100" t="n">
-        <v>0.001548060552408427</v>
-      </c>
-      <c r="G100" t="n">
-        <v>3.750345557868826</v>
+        <v>0.00110847983621849</v>
+      </c>
+      <c r="G100" t="b">
+        <v>0</v>
       </c>
       <c r="H100" t="n">
-        <v>50000</v>
+        <v>1.385599795273113e-05</v>
       </c>
       <c r="I100" t="n">
-        <v>34765.1387839967</v>
-      </c>
-      <c r="J100" t="n">
-        <v>57.07418607842219</v>
-      </c>
-      <c r="K100" t="n">
-        <v>60.82453163629102</v>
-      </c>
-      <c r="L100" t="inlineStr"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
@@ -4300,34 +3554,25 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>183.2270493143958</v>
+        <v>450</v>
       </c>
       <c r="D101" t="n">
-        <v>15298936</v>
+        <v>1002716269.802948</v>
       </c>
       <c r="E101" t="n">
-        <v>523648883.8063354</v>
+        <v>0.002064102610723788</v>
       </c>
       <c r="F101" t="n">
-        <v>0.004736229038808484</v>
-      </c>
-      <c r="G101" t="n">
-        <v>26.76582522771598</v>
+        <v>0.002612294303865996</v>
+      </c>
+      <c r="G101" t="b">
+        <v>0</v>
       </c>
       <c r="H101" t="n">
-        <v>50000</v>
+        <v>3.265367879832495e-05</v>
       </c>
       <c r="I101" t="n">
-        <v>76665.4988758376</v>
-      </c>
-      <c r="J101" t="n">
-        <v>25.88115944061705</v>
-      </c>
-      <c r="K101" t="n">
-        <v>52.64698466833303</v>
-      </c>
-      <c r="L101" t="b">
-        <v>1</v>
+        <v>450</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2024-01-15: Evolved UCB, added volatility
</commit_message>
<xml_diff>
--- a/output/fit_clients/fit_round_1.xlsx
+++ b/output/fit_clients/fit_round_1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I101"/>
+  <dimension ref="A1:J101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,7 +471,12 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>sigmoid</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>g</t>
         </is>
       </c>
     </row>
@@ -485,25 +490,28 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="D2" t="n">
-        <v>10337555872.88031</v>
+        <v>3417482533.119855</v>
       </c>
       <c r="E2" t="n">
-        <v>0.001351815838892293</v>
+        <v>0.004212508431506714</v>
       </c>
       <c r="F2" t="n">
-        <v>0.1203582612079591</v>
+        <v>0.36560509611716</v>
       </c>
       <c r="G2" t="b">
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>0.07345286037387246</v>
+        <v>0.9833950465715571</v>
       </c>
       <c r="I2" t="n">
-        <v>475</v>
+        <v>1</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -516,25 +524,28 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>555</v>
+        <v>601</v>
       </c>
       <c r="D3" t="n">
-        <v>6776767739.039294</v>
+        <v>7090273701.928323</v>
       </c>
       <c r="E3" t="n">
-        <v>0.004891641142873002</v>
+        <v>0.004729482473230561</v>
       </c>
       <c r="F3" t="n">
-        <v>0.2145213626881791</v>
+        <v>0.2220299887114167</v>
       </c>
       <c r="G3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" t="n">
-        <v>0.3883300255292944</v>
+        <v>0.4946317272003546</v>
       </c>
       <c r="I3" t="n">
-        <v>555</v>
+        <v>1</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -547,25 +558,28 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>567</v>
+        <v>500</v>
       </c>
       <c r="D4" t="n">
-        <v>5102461072.54966</v>
+        <v>11255819430.32451</v>
       </c>
       <c r="E4" t="n">
-        <v>0.002660625459979935</v>
+        <v>0.004673846907399744</v>
       </c>
       <c r="F4" t="n">
-        <v>0.2910740736445952</v>
+        <v>0.1163571437963483</v>
       </c>
       <c r="G4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>0.6443188388967274</v>
+        <v>0.1348965935735554</v>
       </c>
       <c r="I4" t="n">
-        <v>567</v>
+        <v>1</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -578,25 +592,28 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>554</v>
+        <v>411</v>
       </c>
       <c r="D5" t="n">
-        <v>3857446537.750169</v>
+        <v>10562344460.68204</v>
       </c>
       <c r="E5" t="n">
-        <v>0.004016583157079982</v>
+        <v>0.001223787715423529</v>
       </c>
       <c r="F5" t="n">
-        <v>0.3761923971722416</v>
+        <v>0.1019252206749639</v>
       </c>
       <c r="G5" t="b">
         <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>0.9289506744442997</v>
+        <v>0.08576694445002181</v>
       </c>
       <c r="I5" t="n">
-        <v>554</v>
+        <v>1</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -609,25 +626,28 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>467</v>
+        <v>514</v>
       </c>
       <c r="D6" t="n">
-        <v>7202066882.010637</v>
+        <v>10318233160.57599</v>
       </c>
       <c r="E6" t="n">
-        <v>0.004860331894281408</v>
+        <v>0.001582336081445277</v>
       </c>
       <c r="F6" t="n">
-        <v>0.1698477881475182</v>
+        <v>0.1304842058758868</v>
       </c>
       <c r="G6" t="b">
         <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>0.2389436067771722</v>
+        <v>0.182988424251734</v>
       </c>
       <c r="I6" t="n">
-        <v>467</v>
+        <v>1</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -640,25 +660,28 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>449</v>
+        <v>612</v>
       </c>
       <c r="D7" t="n">
-        <v>5346299372.838019</v>
+        <v>7389671351.27251</v>
       </c>
       <c r="E7" t="n">
-        <v>0.00476053254405719</v>
+        <v>0.001883725710957506</v>
       </c>
       <c r="F7" t="n">
-        <v>0.2199850827612143</v>
+        <v>0.2169334201478324</v>
       </c>
       <c r="G7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>0.4066004590723261</v>
+        <v>0.4772818131828728</v>
       </c>
       <c r="I7" t="n">
-        <v>449</v>
+        <v>1</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -671,25 +694,28 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>584</v>
+        <v>460</v>
       </c>
       <c r="D8" t="n">
-        <v>9503659139.965311</v>
+        <v>9056376852.383226</v>
       </c>
       <c r="E8" t="n">
-        <v>0.002545926378417389</v>
+        <v>0.00141942319606712</v>
       </c>
       <c r="F8" t="n">
-        <v>0.1609615556988067</v>
+        <v>0.1330465173479304</v>
       </c>
       <c r="G8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>0.2092284461847806</v>
+        <v>0.1917111331040404</v>
       </c>
       <c r="I8" t="n">
-        <v>584</v>
+        <v>1</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -702,25 +728,28 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>444</v>
+        <v>509</v>
       </c>
       <c r="D9" t="n">
-        <v>10606725065.43151</v>
+        <v>7679324230.894574</v>
       </c>
       <c r="E9" t="n">
-        <v>0.004667730463380518</v>
+        <v>0.003457409428442477</v>
       </c>
       <c r="F9" t="n">
-        <v>0.1096482800134393</v>
+        <v>0.1736180775693965</v>
       </c>
       <c r="G9" t="b">
         <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>0.03763916621569262</v>
+        <v>0.3298262340029247</v>
       </c>
       <c r="I9" t="n">
-        <v>444</v>
+        <v>1</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -733,25 +762,28 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>553</v>
+        <v>522</v>
       </c>
       <c r="D10" t="n">
-        <v>10437387192.13124</v>
+        <v>14494107763.26067</v>
       </c>
       <c r="E10" t="n">
-        <v>0.001195970560627643</v>
+        <v>0.002444318691671547</v>
       </c>
       <c r="F10" t="n">
-        <v>0.1387821150385264</v>
+        <v>0.09433637463810328</v>
       </c>
       <c r="G10" t="b">
         <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>0.1350613967773333</v>
+        <v>0.05993273372788778</v>
       </c>
       <c r="I10" t="n">
-        <v>553</v>
+        <v>1</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -764,25 +796,28 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>411</v>
+        <v>579</v>
       </c>
       <c r="D11" t="n">
-        <v>10941590265.81853</v>
+        <v>5567711232.800463</v>
       </c>
       <c r="E11" t="n">
-        <v>0.002341589887010742</v>
+        <v>0.003264219028667802</v>
       </c>
       <c r="F11" t="n">
-        <v>0.09839239670335642</v>
+        <v>0.2723968156008628</v>
       </c>
       <c r="G11" t="b">
         <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>0</v>
+        <v>0.6660922118309631</v>
       </c>
       <c r="I11" t="n">
-        <v>411</v>
+        <v>1</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -795,25 +830,28 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="D12" t="n">
-        <v>7268096986.870382</v>
+        <v>4643083559.058525</v>
       </c>
       <c r="E12" t="n">
-        <v>0.001210634708075548</v>
+        <v>0.001077080645217143</v>
       </c>
       <c r="F12" t="n">
-        <v>0.1744314587835328</v>
+        <v>0.2741763149009815</v>
       </c>
       <c r="G12" t="b">
         <v>0</v>
       </c>
       <c r="H12" t="n">
-        <v>0.2542711946877891</v>
+        <v>0.6721500445601899</v>
       </c>
       <c r="I12" t="n">
-        <v>484</v>
+        <v>1</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -826,25 +864,28 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>473</v>
+        <v>547</v>
       </c>
       <c r="D13" t="n">
-        <v>3968699464.276484</v>
+        <v>5356026622.996432</v>
       </c>
       <c r="E13" t="n">
-        <v>0.003799180704273011</v>
+        <v>0.004896683613022226</v>
       </c>
       <c r="F13" t="n">
-        <v>0.3121857629060535</v>
+        <v>0.2675129215841007</v>
       </c>
       <c r="G13" t="b">
         <v>0</v>
       </c>
       <c r="H13" t="n">
-        <v>0.7149153757757356</v>
+        <v>0.6494662918214176</v>
       </c>
       <c r="I13" t="n">
-        <v>473</v>
+        <v>1</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -857,25 +898,28 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>529</v>
+        <v>615</v>
       </c>
       <c r="D14" t="n">
-        <v>5232293738.2245</v>
+        <v>11787821136.00456</v>
       </c>
       <c r="E14" t="n">
-        <v>0.002083211896376473</v>
+        <v>0.002813756704495657</v>
       </c>
       <c r="F14" t="n">
-        <v>0.2648278898940796</v>
+        <v>0.136660102949782</v>
       </c>
       <c r="G14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" t="n">
-        <v>0.5565527839813988</v>
+        <v>0.2040126255110894</v>
       </c>
       <c r="I14" t="n">
-        <v>529</v>
+        <v>1</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -888,25 +932,28 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>561</v>
+        <v>375</v>
       </c>
       <c r="D15" t="n">
-        <v>8968291691.539831</v>
+        <v>11832489386.08941</v>
       </c>
       <c r="E15" t="n">
-        <v>0.003835257473186202</v>
+        <v>0.001760728831000593</v>
       </c>
       <c r="F15" t="n">
-        <v>0.1638525864838028</v>
+        <v>0.08301475859803301</v>
       </c>
       <c r="G15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" t="n">
-        <v>0.2188959227615566</v>
+        <v>0.0213912989598603</v>
       </c>
       <c r="I15" t="n">
-        <v>561</v>
+        <v>1</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -919,25 +966,28 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>597</v>
+        <v>509</v>
       </c>
       <c r="D16" t="n">
-        <v>4568834457.012507</v>
+        <v>13003589368.81252</v>
       </c>
       <c r="E16" t="n">
-        <v>0.001409256946904231</v>
+        <v>0.004064863544109287</v>
       </c>
       <c r="F16" t="n">
-        <v>0.3422701883189985</v>
+        <v>0.102530883757194</v>
       </c>
       <c r="G16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16" t="n">
-        <v>0.8155163377284145</v>
+        <v>0.08782876354833391</v>
       </c>
       <c r="I16" t="n">
-        <v>597</v>
+        <v>1</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -950,25 +1000,28 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>443</v>
+        <v>548</v>
       </c>
       <c r="D17" t="n">
-        <v>9441907939.574039</v>
+        <v>6382916500.117823</v>
       </c>
       <c r="E17" t="n">
-        <v>0.002632533958853625</v>
+        <v>0.003703471732622985</v>
       </c>
       <c r="F17" t="n">
-        <v>0.1228978059758915</v>
+        <v>0.2248855550552014</v>
       </c>
       <c r="G17" t="b">
         <v>0</v>
       </c>
       <c r="H17" t="n">
-        <v>0.08194498355951146</v>
+        <v>0.5043527443745133</v>
       </c>
       <c r="I17" t="n">
-        <v>443</v>
+        <v>1</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -981,25 +1034,28 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>466</v>
+        <v>419</v>
       </c>
       <c r="D18" t="n">
-        <v>6685959983.656957</v>
+        <v>9624375777.154415</v>
       </c>
       <c r="E18" t="n">
-        <v>0.002530237705619667</v>
+        <v>0.00268396840055083</v>
       </c>
       <c r="F18" t="n">
-        <v>0.1825670125133415</v>
+        <v>0.1140359058511843</v>
       </c>
       <c r="G18" t="b">
         <v>0</v>
       </c>
       <c r="H18" t="n">
-        <v>0.281476119495304</v>
+        <v>0.1269945555139737</v>
       </c>
       <c r="I18" t="n">
-        <v>466</v>
+        <v>1</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -1012,25 +1068,28 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D19" t="n">
-        <v>8545489179.54611</v>
+        <v>11945060301.75842</v>
       </c>
       <c r="E19" t="n">
-        <v>0.003725842327384357</v>
+        <v>0.004381170488033023</v>
       </c>
       <c r="F19" t="n">
-        <v>0.1538746059321372</v>
+        <v>0.1096432304998244</v>
       </c>
       <c r="G19" t="b">
         <v>0</v>
       </c>
       <c r="H19" t="n">
-        <v>0.1855300057442165</v>
+        <v>0.1120408589822805</v>
       </c>
       <c r="I19" t="n">
-        <v>502</v>
+        <v>1</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -1043,25 +1102,28 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>585</v>
+        <v>565</v>
       </c>
       <c r="D20" t="n">
-        <v>8155852843.493005</v>
+        <v>11788767525.29343</v>
       </c>
       <c r="E20" t="n">
-        <v>0.002579420329773804</v>
+        <v>0.00339823203015052</v>
       </c>
       <c r="F20" t="n">
-        <v>0.187882638321822</v>
+        <v>0.1255394464963939</v>
       </c>
       <c r="G20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H20" t="n">
-        <v>0.2992513324958331</v>
+        <v>0.1661553042807147</v>
       </c>
       <c r="I20" t="n">
-        <v>585</v>
+        <v>1</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -1074,25 +1136,28 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>540</v>
+        <v>377</v>
       </c>
       <c r="D21" t="n">
-        <v>11779874268.44426</v>
+        <v>4832184146.39854</v>
       </c>
       <c r="E21" t="n">
-        <v>0.004981914292164171</v>
+        <v>0.002392255091252635</v>
       </c>
       <c r="F21" t="n">
-        <v>0.1200751865229208</v>
+        <v>0.2043610094486978</v>
       </c>
       <c r="G21" t="b">
         <v>0</v>
       </c>
       <c r="H21" t="n">
-        <v>0.07250627139208494</v>
+        <v>0.4344823802112405</v>
       </c>
       <c r="I21" t="n">
-        <v>540</v>
+        <v>1</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -1105,25 +1170,28 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>548</v>
+        <v>604</v>
       </c>
       <c r="D22" t="n">
-        <v>5839989974.722398</v>
+        <v>12734026837.87816</v>
       </c>
       <c r="E22" t="n">
-        <v>0.003435409090929079</v>
+        <v>0.004228785649608674</v>
       </c>
       <c r="F22" t="n">
-        <v>0.2457924972839071</v>
+        <v>0.1242428322275802</v>
       </c>
       <c r="G22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22" t="n">
-        <v>0.4928992894756913</v>
+        <v>0.161741325385484</v>
       </c>
       <c r="I22" t="n">
-        <v>548</v>
+        <v>1</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -1136,25 +1204,28 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>478</v>
+        <v>538</v>
       </c>
       <c r="D23" t="n">
-        <v>9758253162.656689</v>
+        <v>6987454441.414123</v>
       </c>
       <c r="E23" t="n">
-        <v>0.003950282358147591</v>
+        <v>0.00442692559926159</v>
       </c>
       <c r="F23" t="n">
-        <v>0.128308663357031</v>
+        <v>0.2016802874087576</v>
       </c>
       <c r="G23" t="b">
         <v>0</v>
       </c>
       <c r="H23" t="n">
-        <v>0.1000386466446359</v>
+        <v>0.4253565740305771</v>
       </c>
       <c r="I23" t="n">
-        <v>478</v>
+        <v>1</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -1167,25 +1238,28 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>525</v>
+        <v>569</v>
       </c>
       <c r="D24" t="n">
-        <v>8721345098.518131</v>
+        <v>13078082619.62365</v>
       </c>
       <c r="E24" t="n">
-        <v>0.002757449512240559</v>
+        <v>0.004152234714061027</v>
       </c>
       <c r="F24" t="n">
-        <v>0.157679776968539</v>
+        <v>0.1139641760454707</v>
       </c>
       <c r="G24" t="b">
         <v>0</v>
       </c>
       <c r="H24" t="n">
-        <v>0.1982543260994187</v>
+        <v>0.1267503704419794</v>
       </c>
       <c r="I24" t="n">
-        <v>525</v>
+        <v>1</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -1198,25 +1272,28 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>505</v>
+        <v>493</v>
       </c>
       <c r="D25" t="n">
-        <v>5117331076.586716</v>
+        <v>3563506908.307703</v>
       </c>
       <c r="E25" t="n">
-        <v>0.003374091722585616</v>
+        <v>0.003735397575031725</v>
       </c>
       <c r="F25" t="n">
-        <v>0.2584925482058723</v>
+        <v>0.3623843879716966</v>
       </c>
       <c r="G25" t="b">
         <v>0</v>
       </c>
       <c r="H25" t="n">
-        <v>0.5353676870621696</v>
+        <v>0.9724310011158644</v>
       </c>
       <c r="I25" t="n">
-        <v>505</v>
+        <v>1</v>
+      </c>
+      <c r="J25" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -1229,25 +1306,28 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>418</v>
+        <v>591</v>
       </c>
       <c r="D26" t="n">
-        <v>8665710048.940992</v>
+        <v>12230173511.87035</v>
       </c>
       <c r="E26" t="n">
-        <v>0.001619619687924144</v>
+        <v>0.003346233460880628</v>
       </c>
       <c r="F26" t="n">
-        <v>0.126349140903209</v>
+        <v>0.1265770668337195</v>
       </c>
       <c r="G26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26" t="n">
-        <v>0.09348609192183442</v>
+        <v>0.1696876071254212</v>
       </c>
       <c r="I26" t="n">
-        <v>418</v>
+        <v>1</v>
+      </c>
+      <c r="J26" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -1260,25 +1340,28 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>559</v>
+        <v>587</v>
       </c>
       <c r="D27" t="n">
-        <v>9921210566.358397</v>
+        <v>11761528792.5984</v>
       </c>
       <c r="E27" t="n">
-        <v>0.001976772246546785</v>
+        <v>0.00401423750995453</v>
       </c>
       <c r="F27" t="n">
-        <v>0.1475867284749559</v>
+        <v>0.130729767967546</v>
       </c>
       <c r="G27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H27" t="n">
-        <v>0.1645036270731845</v>
+        <v>0.1838243751710803</v>
       </c>
       <c r="I27" t="n">
-        <v>559</v>
+        <v>1</v>
+      </c>
+      <c r="J27" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -1291,25 +1374,28 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>440</v>
+        <v>578</v>
       </c>
       <c r="D28" t="n">
-        <v>7195299205.473581</v>
+        <v>6585679997.160779</v>
       </c>
       <c r="E28" t="n">
-        <v>0.004708951780596967</v>
+        <v>0.003820774004081493</v>
       </c>
       <c r="F28" t="n">
-        <v>0.160178411916943</v>
+        <v>0.2298938637548013</v>
       </c>
       <c r="G28" t="b">
         <v>0</v>
       </c>
       <c r="H28" t="n">
-        <v>0.2066096486933435</v>
+        <v>0.5214022011270296</v>
       </c>
       <c r="I28" t="n">
-        <v>440</v>
+        <v>1</v>
+      </c>
+      <c r="J28" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -1322,25 +1408,28 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>521</v>
+        <v>618</v>
       </c>
       <c r="D29" t="n">
-        <v>9024823093.212418</v>
+        <v>10629542131.70882</v>
       </c>
       <c r="E29" t="n">
-        <v>0.003648709149239378</v>
+        <v>0.004965611296417732</v>
       </c>
       <c r="F29" t="n">
-        <v>0.151216503182915</v>
+        <v>0.1522909453617042</v>
       </c>
       <c r="G29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H29" t="n">
-        <v>0.1766414300154027</v>
+        <v>0.2572236769242652</v>
       </c>
       <c r="I29" t="n">
-        <v>521</v>
+        <v>1</v>
+      </c>
+      <c r="J29" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -1353,25 +1442,28 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>588</v>
+        <v>477</v>
       </c>
       <c r="D30" t="n">
-        <v>11100488798.10759</v>
+        <v>4141216514.382464</v>
       </c>
       <c r="E30" t="n">
-        <v>0.003692672530015469</v>
+        <v>0.004754256667193547</v>
       </c>
       <c r="F30" t="n">
-        <v>0.138750765665614</v>
+        <v>0.3017106267350808</v>
       </c>
       <c r="G30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H30" t="n">
-        <v>0.134956565887984</v>
+        <v>0.7658832960395325</v>
       </c>
       <c r="I30" t="n">
-        <v>588</v>
+        <v>1</v>
+      </c>
+      <c r="J30" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -1384,25 +1476,28 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>562</v>
+        <v>375</v>
       </c>
       <c r="D31" t="n">
-        <v>8967914304.384113</v>
+        <v>5540027361.456321</v>
       </c>
       <c r="E31" t="n">
-        <v>0.004953000027454639</v>
+        <v>0.00204219693722102</v>
       </c>
       <c r="F31" t="n">
-        <v>0.16415156635477</v>
+        <v>0.1773044040962621</v>
       </c>
       <c r="G31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H31" t="n">
-        <v>0.2198956979678616</v>
+        <v>0.3423753535690708</v>
       </c>
       <c r="I31" t="n">
-        <v>562</v>
+        <v>1</v>
+      </c>
+      <c r="J31" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -1415,25 +1510,28 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>448</v>
+        <v>397</v>
       </c>
       <c r="D32" t="n">
-        <v>5738357601.584291</v>
+        <v>10552502884.23811</v>
       </c>
       <c r="E32" t="n">
-        <v>0.002302539363220608</v>
+        <v>0.003322977913475706</v>
       </c>
       <c r="F32" t="n">
-        <v>0.2044987087727008</v>
+        <v>0.0985451358230148</v>
       </c>
       <c r="G32" t="b">
         <v>0</v>
       </c>
       <c r="H32" t="n">
-        <v>0.354814722797867</v>
+        <v>0.07426034332782142</v>
       </c>
       <c r="I32" t="n">
-        <v>448</v>
+        <v>1</v>
+      </c>
+      <c r="J32" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -1446,25 +1544,28 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>419</v>
+        <v>519</v>
       </c>
       <c r="D33" t="n">
-        <v>6117692558.508032</v>
+        <v>8825291703.487873</v>
       </c>
       <c r="E33" t="n">
-        <v>0.003042729667140085</v>
+        <v>0.003449276237456637</v>
       </c>
       <c r="F33" t="n">
-        <v>0.1794016942668432</v>
+        <v>0.1540417535958298</v>
       </c>
       <c r="G33" t="b">
         <v>0</v>
       </c>
       <c r="H33" t="n">
-        <v>0.2708914380159937</v>
+        <v>0.2631838385397141</v>
       </c>
       <c r="I33" t="n">
-        <v>419</v>
+        <v>1</v>
+      </c>
+      <c r="J33" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -1477,25 +1578,28 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>537</v>
+        <v>424</v>
       </c>
       <c r="D34" t="n">
-        <v>9470764724.801638</v>
+        <v>10246400528.88758</v>
       </c>
       <c r="E34" t="n">
-        <v>0.00168172816104123</v>
+        <v>0.004010447019284172</v>
       </c>
       <c r="F34" t="n">
-        <v>0.1485215260723797</v>
+        <v>0.1083913669848095</v>
       </c>
       <c r="G34" t="b">
         <v>0</v>
       </c>
       <c r="H34" t="n">
-        <v>0.1676295480851717</v>
+        <v>0.1077792221424819</v>
       </c>
       <c r="I34" t="n">
-        <v>537</v>
+        <v>1</v>
+      </c>
+      <c r="J34" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -1508,25 +1612,28 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>474</v>
+        <v>611</v>
       </c>
       <c r="D35" t="n">
-        <v>5242980849.401595</v>
+        <v>7766220700.608027</v>
       </c>
       <c r="E35" t="n">
-        <v>0.002295289182122432</v>
+        <v>0.00487487922544918</v>
       </c>
       <c r="F35" t="n">
-        <v>0.2368101077732734</v>
+        <v>0.2060780077850091</v>
       </c>
       <c r="G35" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H35" t="n">
-        <v>0.4628625840043417</v>
+        <v>0.4403274450095466</v>
       </c>
       <c r="I35" t="n">
-        <v>474</v>
+        <v>1</v>
+      </c>
+      <c r="J35" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -1539,25 +1646,28 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>590</v>
+        <v>463</v>
       </c>
       <c r="D36" t="n">
-        <v>10826697104.62261</v>
+        <v>11387238210.29493</v>
       </c>
       <c r="E36" t="n">
-        <v>0.0016731837889433</v>
+        <v>0.004396834918372778</v>
       </c>
       <c r="F36" t="n">
-        <v>0.1427434502938253</v>
+        <v>0.1065032229591506</v>
       </c>
       <c r="G36" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H36" t="n">
-        <v>0.1483079232384518</v>
+        <v>0.1013515373013765</v>
       </c>
       <c r="I36" t="n">
-        <v>590</v>
+        <v>1</v>
+      </c>
+      <c r="J36" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -1570,25 +1680,28 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>459</v>
+        <v>378</v>
       </c>
       <c r="D37" t="n">
-        <v>8265822884.832561</v>
+        <v>4537413214.182314</v>
       </c>
       <c r="E37" t="n">
-        <v>0.003464404985076307</v>
+        <v>0.003463822825190348</v>
       </c>
       <c r="F37" t="n">
-        <v>0.1454543639213671</v>
+        <v>0.2182145141432597</v>
       </c>
       <c r="G37" t="b">
         <v>0</v>
       </c>
       <c r="H37" t="n">
-        <v>0.1573730961629109</v>
+        <v>0.4816429574295706</v>
       </c>
       <c r="I37" t="n">
-        <v>459</v>
+        <v>1</v>
+      </c>
+      <c r="J37" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -1601,25 +1714,28 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>409</v>
+        <v>481</v>
       </c>
       <c r="D38" t="n">
-        <v>9150625701.224808</v>
+        <v>5530498844.961464</v>
       </c>
       <c r="E38" t="n">
-        <v>0.001880144056847697</v>
+        <v>0.002473299080977689</v>
       </c>
       <c r="F38" t="n">
-        <v>0.1170772955839078</v>
+        <v>0.2278142759486968</v>
       </c>
       <c r="G38" t="b">
         <v>0</v>
       </c>
       <c r="H38" t="n">
-        <v>0.06248145927903193</v>
+        <v>0.5143227967831898</v>
       </c>
       <c r="I38" t="n">
-        <v>409</v>
+        <v>1</v>
+      </c>
+      <c r="J38" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -1632,25 +1748,28 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>445</v>
+        <v>573</v>
       </c>
       <c r="D39" t="n">
-        <v>7302065352.58524</v>
+        <v>5508749317.826727</v>
       </c>
       <c r="E39" t="n">
-        <v>0.003428804882655717</v>
+        <v>0.003401184631037176</v>
       </c>
       <c r="F39" t="n">
-        <v>0.1596299805215134</v>
+        <v>0.2724593884029068</v>
       </c>
       <c r="G39" t="b">
         <v>0</v>
       </c>
       <c r="H39" t="n">
-        <v>0.2047757188380129</v>
+        <v>0.6663052243160799</v>
       </c>
       <c r="I39" t="n">
-        <v>445</v>
+        <v>1</v>
+      </c>
+      <c r="J39" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -1663,25 +1782,28 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D40" t="n">
-        <v>5207780676.166952</v>
+        <v>8751420130.836655</v>
       </c>
       <c r="E40" t="n">
-        <v>0.003944419583593229</v>
+        <v>0.002234513778143185</v>
       </c>
       <c r="F40" t="n">
-        <v>0.2675833654779909</v>
+        <v>0.1589337580879033</v>
       </c>
       <c r="G40" t="b">
         <v>0</v>
       </c>
       <c r="H40" t="n">
-        <v>0.5657669700784788</v>
+        <v>0.2798373685083014</v>
       </c>
       <c r="I40" t="n">
-        <v>532</v>
+        <v>1</v>
+      </c>
+      <c r="J40" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="41">
@@ -1694,25 +1816,28 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>489</v>
+        <v>448</v>
       </c>
       <c r="D41" t="n">
-        <v>3907102328.760626</v>
+        <v>5006504821.185925</v>
       </c>
       <c r="E41" t="n">
-        <v>0.001532106934649001</v>
+        <v>0.00219550369589986</v>
       </c>
       <c r="F41" t="n">
-        <v>0.3278341855986938</v>
+        <v>0.2343924078599066</v>
       </c>
       <c r="G41" t="b">
         <v>0</v>
       </c>
       <c r="H41" t="n">
-        <v>0.7672429956093644</v>
+        <v>0.5367162997119289</v>
       </c>
       <c r="I41" t="n">
-        <v>489</v>
+        <v>1</v>
+      </c>
+      <c r="J41" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -1725,25 +1850,28 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>465</v>
+        <v>432</v>
       </c>
       <c r="D42" t="n">
-        <v>5608327073.618356</v>
+        <v>8402711629.809205</v>
       </c>
       <c r="E42" t="n">
-        <v>0.001144279356828981</v>
+        <v>0.004753020793672395</v>
       </c>
       <c r="F42" t="n">
-        <v>0.217179977917045</v>
+        <v>0.1346680131192</v>
       </c>
       <c r="G42" t="b">
         <v>0</v>
       </c>
       <c r="H42" t="n">
-        <v>0.3972203149669269</v>
+        <v>0.197231084785305</v>
       </c>
       <c r="I42" t="n">
-        <v>465</v>
+        <v>1</v>
+      </c>
+      <c r="J42" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -1756,25 +1884,28 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>487</v>
+        <v>378</v>
       </c>
       <c r="D43" t="n">
-        <v>8058703391.396841</v>
+        <v>3691172050.662078</v>
       </c>
       <c r="E43" t="n">
-        <v>0.004111428154496694</v>
+        <v>0.003894510149731226</v>
       </c>
       <c r="F43" t="n">
-        <v>0.1582938182539175</v>
+        <v>0.268242554508507</v>
       </c>
       <c r="G43" t="b">
         <v>0</v>
       </c>
       <c r="H43" t="n">
-        <v>0.2003076524681235</v>
+        <v>0.6519501333208186</v>
       </c>
       <c r="I43" t="n">
-        <v>487</v>
+        <v>1</v>
+      </c>
+      <c r="J43" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -1787,25 +1918,28 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>575</v>
+        <v>589</v>
       </c>
       <c r="D44" t="n">
-        <v>5512153893.453278</v>
+        <v>13607867046.35512</v>
       </c>
       <c r="E44" t="n">
-        <v>0.001635809515497397</v>
+        <v>0.00239899485333726</v>
       </c>
       <c r="F44" t="n">
-        <v>0.2732415094195458</v>
+        <v>0.1133771152190414</v>
       </c>
       <c r="G44" t="b">
         <v>1</v>
       </c>
       <c r="H44" t="n">
-        <v>0.5846875482704831</v>
+        <v>0.1247518777827504</v>
       </c>
       <c r="I44" t="n">
-        <v>575</v>
+        <v>1</v>
+      </c>
+      <c r="J44" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="45">
@@ -1818,25 +1952,28 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>598</v>
+        <v>376</v>
       </c>
       <c r="D45" t="n">
-        <v>7109812108.699032</v>
+        <v>8311377798.971918</v>
       </c>
       <c r="E45" t="n">
-        <v>0.001034802239271949</v>
+        <v>0.001818596851300997</v>
       </c>
       <c r="F45" t="n">
-        <v>0.2203145731634</v>
+        <v>0.118499082080209</v>
       </c>
       <c r="G45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H45" t="n">
-        <v>0.4077022601191823</v>
+        <v>0.142188253558524</v>
       </c>
       <c r="I45" t="n">
-        <v>598</v>
+        <v>1</v>
+      </c>
+      <c r="J45" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="46">
@@ -1849,25 +1986,28 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>410</v>
+        <v>594</v>
       </c>
       <c r="D46" t="n">
-        <v>7629119701.953492</v>
+        <v>6844757309.321449</v>
       </c>
       <c r="E46" t="n">
-        <v>0.002323942061119299</v>
+        <v>0.001716169518917231</v>
       </c>
       <c r="F46" t="n">
-        <v>0.1407698321635991</v>
+        <v>0.2273152413864393</v>
       </c>
       <c r="G46" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H46" t="n">
-        <v>0.1417082332093855</v>
+        <v>0.5126239661604088</v>
       </c>
       <c r="I46" t="n">
-        <v>410</v>
+        <v>1</v>
+      </c>
+      <c r="J46" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -1880,25 +2020,28 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>475</v>
+        <v>419</v>
       </c>
       <c r="D47" t="n">
-        <v>8859934516.80341</v>
+        <v>3305332026.108679</v>
       </c>
       <c r="E47" t="n">
-        <v>0.004545676530028684</v>
+        <v>0.003104837579760703</v>
       </c>
       <c r="F47" t="n">
-        <v>0.1404310886993893</v>
+        <v>0.3320466450361721</v>
       </c>
       <c r="G47" t="b">
         <v>0</v>
       </c>
       <c r="H47" t="n">
-        <v>0.1405754903403784</v>
+        <v>0.8691542130477674</v>
       </c>
       <c r="I47" t="n">
-        <v>475</v>
+        <v>1</v>
+      </c>
+      <c r="J47" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="48">
@@ -1911,25 +2054,28 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="D48" t="n">
-        <v>7735748053.356518</v>
+        <v>10446671618.84252</v>
       </c>
       <c r="E48" t="n">
-        <v>0.004913119409870457</v>
+        <v>0.004633460584861609</v>
       </c>
       <c r="F48" t="n">
-        <v>0.1980859691177663</v>
+        <v>0.146180948891471</v>
       </c>
       <c r="G48" t="b">
         <v>1</v>
       </c>
       <c r="H48" t="n">
-        <v>0.3333708105680888</v>
+        <v>0.2364238167667653</v>
       </c>
       <c r="I48" t="n">
-        <v>585</v>
+        <v>1</v>
+      </c>
+      <c r="J48" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="49">
@@ -1942,25 +2088,28 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>440</v>
+        <v>431</v>
       </c>
       <c r="D49" t="n">
-        <v>7486813771.556484</v>
+        <v>8604503232.453457</v>
       </c>
       <c r="E49" t="n">
-        <v>0.003272627013291664</v>
+        <v>0.001218675383278662</v>
       </c>
       <c r="F49" t="n">
-        <v>0.1539415344319954</v>
+        <v>0.1312053769405225</v>
       </c>
       <c r="G49" t="b">
         <v>0</v>
       </c>
       <c r="H49" t="n">
-        <v>0.1857538116296663</v>
+        <v>0.1854434595970301</v>
       </c>
       <c r="I49" t="n">
-        <v>440</v>
+        <v>1</v>
+      </c>
+      <c r="J49" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="50">
@@ -1973,25 +2122,28 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>529</v>
+        <v>521</v>
       </c>
       <c r="D50" t="n">
-        <v>4292662757.473536</v>
+        <v>4814310362.881804</v>
       </c>
       <c r="E50" t="n">
-        <v>0.004131512628833012</v>
+        <v>0.003098710838858551</v>
       </c>
       <c r="F50" t="n">
-        <v>0.3227966854809564</v>
+        <v>0.2834678463029336</v>
       </c>
       <c r="G50" t="b">
         <v>0</v>
       </c>
       <c r="H50" t="n">
-        <v>0.7503978223768698</v>
+        <v>0.7037805953716618</v>
       </c>
       <c r="I50" t="n">
-        <v>529</v>
+        <v>1</v>
+      </c>
+      <c r="J50" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="51">
@@ -2004,25 +2156,28 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>477</v>
+        <v>514</v>
       </c>
       <c r="D51" t="n">
-        <v>10561154963.5492</v>
+        <v>9374706022.480885</v>
       </c>
       <c r="E51" t="n">
-        <v>0.002903440489956149</v>
+        <v>0.003893258485698142</v>
       </c>
       <c r="F51" t="n">
-        <v>0.1183060976107587</v>
+        <v>0.1436169258824079</v>
       </c>
       <c r="G51" t="b">
         <v>0</v>
       </c>
       <c r="H51" t="n">
-        <v>0.06659051784517664</v>
+        <v>0.2276952814412628</v>
       </c>
       <c r="I51" t="n">
-        <v>477</v>
+        <v>1</v>
+      </c>
+      <c r="J51" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="52">
@@ -2035,25 +2190,28 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>535</v>
+        <v>428</v>
       </c>
       <c r="D52" t="n">
-        <v>4853837140.267541</v>
+        <v>13000197621.17138</v>
       </c>
       <c r="E52" t="n">
-        <v>0.0032647394106087</v>
+        <v>0.002978364556538109</v>
       </c>
       <c r="F52" t="n">
-        <v>0.2887146003260334</v>
+        <v>0.08623706751766931</v>
       </c>
       <c r="G52" t="b">
         <v>0</v>
       </c>
       <c r="H52" t="n">
-        <v>0.6364288665176352</v>
+        <v>0.03236079382605653</v>
       </c>
       <c r="I52" t="n">
-        <v>535</v>
+        <v>1</v>
+      </c>
+      <c r="J52" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="53">
@@ -2066,25 +2224,28 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>455</v>
+        <v>528</v>
       </c>
       <c r="D53" t="n">
-        <v>5809656670.864542</v>
+        <v>5497834204.272991</v>
       </c>
       <c r="E53" t="n">
-        <v>0.001614771459233107</v>
+        <v>0.004748837903182749</v>
       </c>
       <c r="F53" t="n">
-        <v>0.2051450744029326</v>
+        <v>0.2515604997555372</v>
       </c>
       <c r="G53" t="b">
         <v>0</v>
       </c>
       <c r="H53" t="n">
-        <v>0.3569761403181259</v>
+        <v>0.5951605086963242</v>
       </c>
       <c r="I53" t="n">
-        <v>455</v>
+        <v>1</v>
+      </c>
+      <c r="J53" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="54">
@@ -2097,25 +2258,28 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>553</v>
+        <v>608</v>
       </c>
       <c r="D54" t="n">
-        <v>8607190525.755182</v>
+        <v>12661786413.6946</v>
       </c>
       <c r="E54" t="n">
-        <v>0.004702064893980365</v>
+        <v>0.003825806088110311</v>
       </c>
       <c r="F54" t="n">
-        <v>0.1682921582443894</v>
+        <v>0.1257791805963102</v>
       </c>
       <c r="G54" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H54" t="n">
-        <v>0.2337416505307426</v>
+        <v>0.1669714153500969</v>
       </c>
       <c r="I54" t="n">
-        <v>553</v>
+        <v>1</v>
+      </c>
+      <c r="J54" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="55">
@@ -2128,25 +2292,28 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>567</v>
+        <v>505</v>
       </c>
       <c r="D55" t="n">
-        <v>9348029578.087059</v>
+        <v>6039426530.770609</v>
       </c>
       <c r="E55" t="n">
-        <v>0.001483566800546472</v>
+        <v>0.001561774962723762</v>
       </c>
       <c r="F55" t="n">
-        <v>0.1588777739301852</v>
+        <v>0.2190260852185938</v>
       </c>
       <c r="G55" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H55" t="n">
-        <v>0.2022603739166435</v>
+        <v>0.4844057356008938</v>
       </c>
       <c r="I55" t="n">
-        <v>567</v>
+        <v>1</v>
+      </c>
+      <c r="J55" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -2159,25 +2326,28 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>586</v>
+        <v>478</v>
       </c>
       <c r="D56" t="n">
-        <v>4699916888.55228</v>
+        <v>10360331607.939</v>
       </c>
       <c r="E56" t="n">
-        <v>0.001146718870240128</v>
+        <v>0.004915031371577813</v>
       </c>
       <c r="F56" t="n">
-        <v>0.3265935497154751</v>
+        <v>0.1208521568016756</v>
       </c>
       <c r="G56" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H56" t="n">
-        <v>0.7630943651611619</v>
+        <v>0.1501986714671265</v>
       </c>
       <c r="I56" t="n">
-        <v>586</v>
+        <v>1</v>
+      </c>
+      <c r="J56" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="57">
@@ -2190,25 +2360,28 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>417</v>
+        <v>376</v>
       </c>
       <c r="D57" t="n">
-        <v>5846302768.190098</v>
+        <v>12835624550.76095</v>
       </c>
       <c r="E57" t="n">
-        <v>0.001892700453050512</v>
+        <v>0.002277044999587436</v>
       </c>
       <c r="F57" t="n">
-        <v>0.1868335721412099</v>
+        <v>0.07673102591191101</v>
       </c>
       <c r="G57" t="b">
         <v>0</v>
       </c>
       <c r="H57" t="n">
-        <v>0.295743302494496</v>
+        <v>0</v>
       </c>
       <c r="I57" t="n">
-        <v>417</v>
+        <v>1</v>
+      </c>
+      <c r="J57" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="58">
@@ -2221,25 +2394,28 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>435</v>
+        <v>618</v>
       </c>
       <c r="D58" t="n">
-        <v>5977312554.086927</v>
+        <v>11920825727.53852</v>
       </c>
       <c r="E58" t="n">
-        <v>0.003599858423189042</v>
+        <v>0.003210105022742737</v>
       </c>
       <c r="F58" t="n">
-        <v>0.1906265800373653</v>
+        <v>0.1357945378112876</v>
       </c>
       <c r="G58" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H58" t="n">
-        <v>0.3084269498571991</v>
+        <v>0.2010660388926516</v>
       </c>
       <c r="I58" t="n">
-        <v>435</v>
+        <v>1</v>
+      </c>
+      <c r="J58" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="59">
@@ -2252,25 +2428,28 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>520</v>
+        <v>603</v>
       </c>
       <c r="D59" t="n">
-        <v>4465928626.48337</v>
+        <v>8022708876.786443</v>
       </c>
       <c r="E59" t="n">
-        <v>0.002381176626755057</v>
+        <v>0.001921373897318952</v>
       </c>
       <c r="F59" t="n">
-        <v>0.3049943055342898</v>
+        <v>0.1968776624277407</v>
       </c>
       <c r="G59" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H59" t="n">
-        <v>0.6908674666164066</v>
+        <v>0.4090073128680325</v>
       </c>
       <c r="I59" t="n">
-        <v>520</v>
+        <v>1</v>
+      </c>
+      <c r="J59" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="60">
@@ -2283,25 +2462,28 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>586</v>
+        <v>388</v>
       </c>
       <c r="D60" t="n">
-        <v>3862128883.89255</v>
+        <v>12775714417.31358</v>
       </c>
       <c r="E60" t="n">
-        <v>0.004383659442112248</v>
+        <v>0.004442299867078091</v>
       </c>
       <c r="F60" t="n">
-        <v>0.3974394915720541</v>
+        <v>0.07955119273977226</v>
       </c>
       <c r="G60" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H60" t="n">
-        <v>1</v>
+        <v>0.009600508924368603</v>
       </c>
       <c r="I60" t="n">
-        <v>586</v>
+        <v>1</v>
+      </c>
+      <c r="J60" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="61">
@@ -2314,25 +2496,28 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>404</v>
+        <v>383</v>
       </c>
       <c r="D61" t="n">
-        <v>7247114824.87918</v>
+        <v>8372217478.321583</v>
       </c>
       <c r="E61" t="n">
-        <v>0.00241419510991461</v>
+        <v>0.002019913043639493</v>
       </c>
       <c r="F61" t="n">
-        <v>0.1460213596129467</v>
+        <v>0.1198280351170621</v>
       </c>
       <c r="G61" t="b">
         <v>0</v>
       </c>
       <c r="H61" t="n">
-        <v>0.159269104187428</v>
+        <v>0.1467123212003136</v>
       </c>
       <c r="I61" t="n">
-        <v>404</v>
+        <v>1</v>
+      </c>
+      <c r="J61" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="62">
@@ -2345,25 +2530,28 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>575</v>
+        <v>582</v>
       </c>
       <c r="D62" t="n">
-        <v>8709483512.159214</v>
+        <v>7359096118.678984</v>
       </c>
       <c r="E62" t="n">
-        <v>0.003758092146377222</v>
+        <v>0.003771226796759389</v>
       </c>
       <c r="F62" t="n">
-        <v>0.1729320972819205</v>
+        <v>0.2071565523013792</v>
       </c>
       <c r="G62" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H62" t="n">
-        <v>0.2492573974386615</v>
+        <v>0.4439990633522788</v>
       </c>
       <c r="I62" t="n">
-        <v>575</v>
+        <v>1</v>
+      </c>
+      <c r="J62" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="63">
@@ -2376,25 +2564,28 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>561</v>
+        <v>596</v>
       </c>
       <c r="D63" t="n">
-        <v>9488719094.379845</v>
+        <v>8487164941.822082</v>
       </c>
       <c r="E63" t="n">
-        <v>0.001541526426544644</v>
+        <v>0.002427678262990123</v>
       </c>
       <c r="F63" t="n">
-        <v>0.1548657701196329</v>
+        <v>0.1839432190491682</v>
       </c>
       <c r="G63" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H63" t="n">
-        <v>0.1888444140916071</v>
+        <v>0.3649754357957464</v>
       </c>
       <c r="I63" t="n">
-        <v>561</v>
+        <v>1</v>
+      </c>
+      <c r="J63" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="64">
@@ -2407,25 +2598,28 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>522</v>
+        <v>476</v>
       </c>
       <c r="D64" t="n">
-        <v>7727366757.286109</v>
+        <v>14824503195.70986</v>
       </c>
       <c r="E64" t="n">
-        <v>0.001804699437831559</v>
+        <v>0.004610314179341419</v>
       </c>
       <c r="F64" t="n">
-        <v>0.1769453454128804</v>
+        <v>0.08410599826109695</v>
       </c>
       <c r="G64" t="b">
         <v>0</v>
       </c>
       <c r="H64" t="n">
-        <v>0.2626775182150294</v>
+        <v>0.02510613455765913</v>
       </c>
       <c r="I64" t="n">
-        <v>522</v>
+        <v>1</v>
+      </c>
+      <c r="J64" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="65">
@@ -2438,25 +2632,28 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>461</v>
+        <v>383</v>
       </c>
       <c r="D65" t="n">
-        <v>7642119846.766719</v>
+        <v>10296948678.99721</v>
       </c>
       <c r="E65" t="n">
-        <v>0.00233644233676065</v>
+        <v>0.004978969050527762</v>
       </c>
       <c r="F65" t="n">
-        <v>0.1580109726375063</v>
+        <v>0.0974294814197036</v>
       </c>
       <c r="G65" t="b">
         <v>0</v>
       </c>
       <c r="H65" t="n">
-        <v>0.1993618294814955</v>
+        <v>0.07046239423144716</v>
       </c>
       <c r="I65" t="n">
-        <v>461</v>
+        <v>1</v>
+      </c>
+      <c r="J65" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="66">
@@ -2469,25 +2666,28 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="D66" t="n">
-        <v>8476676139.201751</v>
+        <v>9065314311.780197</v>
       </c>
       <c r="E66" t="n">
-        <v>0.001461693853076115</v>
+        <v>0.004938173837721294</v>
       </c>
       <c r="F66" t="n">
-        <v>0.1452353823341815</v>
+        <v>0.1343600793209356</v>
       </c>
       <c r="G66" t="b">
         <v>0</v>
       </c>
       <c r="H66" t="n">
-        <v>0.1566408316101262</v>
+        <v>0.1961828059568523</v>
       </c>
       <c r="I66" t="n">
-        <v>470</v>
+        <v>1</v>
+      </c>
+      <c r="J66" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="67">
@@ -2500,25 +2700,28 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>459</v>
+        <v>385</v>
       </c>
       <c r="D67" t="n">
-        <v>4750619615.408079</v>
+        <v>6056467473.27987</v>
       </c>
       <c r="E67" t="n">
-        <v>0.004617733709396809</v>
+        <v>0.001302970660678709</v>
       </c>
       <c r="F67" t="n">
-        <v>0.2530827781076137</v>
+        <v>0.1665104542291659</v>
       </c>
       <c r="G67" t="b">
         <v>0</v>
       </c>
       <c r="H67" t="n">
-        <v>0.5172776598019688</v>
+        <v>0.3056302181379049</v>
       </c>
       <c r="I67" t="n">
-        <v>459</v>
+        <v>1</v>
+      </c>
+      <c r="J67" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="68">
@@ -2531,25 +2734,28 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>446</v>
+        <v>513</v>
       </c>
       <c r="D68" t="n">
-        <v>8601409296.903402</v>
+        <v>9352523719.545055</v>
       </c>
       <c r="E68" t="n">
-        <v>0.004903775497223803</v>
+        <v>0.002442647305339544</v>
       </c>
       <c r="F68" t="n">
-        <v>0.1358205265758695</v>
+        <v>0.1436774832435672</v>
       </c>
       <c r="G68" t="b">
         <v>0</v>
       </c>
       <c r="H68" t="n">
-        <v>0.12515797850819</v>
+        <v>0.2279014328931922</v>
       </c>
       <c r="I68" t="n">
-        <v>446</v>
+        <v>1</v>
+      </c>
+      <c r="J68" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="69">
@@ -2562,25 +2768,28 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>544</v>
+        <v>470</v>
       </c>
       <c r="D69" t="n">
-        <v>6737951918.720098</v>
+        <v>6144271904.914864</v>
       </c>
       <c r="E69" t="n">
-        <v>0.001009454970858385</v>
+        <v>0.001473085525823155</v>
       </c>
       <c r="F69" t="n">
-        <v>0.2114809035726505</v>
+        <v>0.200367646330108</v>
       </c>
       <c r="G69" t="b">
         <v>0</v>
       </c>
       <c r="H69" t="n">
-        <v>0.3781628673535441</v>
+        <v>0.4208880361180076</v>
       </c>
       <c r="I69" t="n">
-        <v>544</v>
+        <v>1</v>
+      </c>
+      <c r="J69" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="70">
@@ -2593,25 +2802,28 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>507</v>
+        <v>403</v>
       </c>
       <c r="D70" t="n">
-        <v>9636512440.990805</v>
+        <v>7940544763.928969</v>
       </c>
       <c r="E70" t="n">
-        <v>0.002152856045830613</v>
+        <v>0.002059327837050325</v>
       </c>
       <c r="F70" t="n">
-        <v>0.1378123816196158</v>
+        <v>0.1329397669030561</v>
       </c>
       <c r="G70" t="b">
         <v>0</v>
       </c>
       <c r="H70" t="n">
-        <v>0.1318186519536913</v>
+        <v>0.1913477295675649</v>
       </c>
       <c r="I70" t="n">
-        <v>507</v>
+        <v>1</v>
+      </c>
+      <c r="J70" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="71">
@@ -2624,25 +2836,28 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>417</v>
+        <v>573</v>
       </c>
       <c r="D71" t="n">
-        <v>10958117928.18942</v>
+        <v>5936001024.128036</v>
       </c>
       <c r="E71" t="n">
-        <v>0.004135454195375603</v>
+        <v>0.002557261864882081</v>
       </c>
       <c r="F71" t="n">
-        <v>0.09967821455818873</v>
+        <v>0.2528487552308795</v>
       </c>
       <c r="G71" t="b">
         <v>0</v>
       </c>
       <c r="H71" t="n">
-        <v>0.00429971692384062</v>
+        <v>0.5995460322992913</v>
       </c>
       <c r="I71" t="n">
-        <v>417</v>
+        <v>1</v>
+      </c>
+      <c r="J71" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="72">
@@ -2655,25 +2870,28 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>467</v>
+        <v>532</v>
       </c>
       <c r="D72" t="n">
-        <v>6793831797.503946</v>
+        <v>3761349684.21081</v>
       </c>
       <c r="E72" t="n">
-        <v>0.00148032754405016</v>
+        <v>0.001994795644767385</v>
       </c>
       <c r="F72" t="n">
-        <v>0.1800537850303306</v>
+        <v>0.3704828311628732</v>
       </c>
       <c r="G72" t="b">
         <v>0</v>
       </c>
       <c r="H72" t="n">
-        <v>0.2730720001236901</v>
+        <v>1</v>
       </c>
       <c r="I72" t="n">
-        <v>467</v>
+        <v>1</v>
+      </c>
+      <c r="J72" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="73">
@@ -2686,25 +2904,28 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>509</v>
+        <v>571</v>
       </c>
       <c r="D73" t="n">
-        <v>4897937761.529299</v>
+        <v>6508499003.969236</v>
       </c>
       <c r="E73" t="n">
-        <v>0.004150488471087899</v>
+        <v>0.003990783982156835</v>
       </c>
       <c r="F73" t="n">
-        <v>0.272210382188219</v>
+        <v>0.2298028607038056</v>
       </c>
       <c r="G73" t="b">
         <v>0</v>
       </c>
       <c r="H73" t="n">
-        <v>0.5812395053066162</v>
+        <v>0.5210924054104795</v>
       </c>
       <c r="I73" t="n">
-        <v>509</v>
+        <v>1</v>
+      </c>
+      <c r="J73" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="74">
@@ -2717,25 +2938,28 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>453</v>
+        <v>388</v>
       </c>
       <c r="D74" t="n">
-        <v>9259613998.581919</v>
+        <v>8074694279.648926</v>
       </c>
       <c r="E74" t="n">
-        <v>0.001253580176352478</v>
+        <v>0.00196962289377296</v>
       </c>
       <c r="F74" t="n">
-        <v>0.1281461268452142</v>
+        <v>0.1258652383362046</v>
       </c>
       <c r="G74" t="b">
         <v>0</v>
       </c>
       <c r="H74" t="n">
-        <v>0.09949513187854826</v>
+        <v>0.167264376068486</v>
       </c>
       <c r="I74" t="n">
-        <v>453</v>
+        <v>1</v>
+      </c>
+      <c r="J74" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="75">
@@ -2748,25 +2972,28 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>568</v>
+        <v>396</v>
       </c>
       <c r="D75" t="n">
-        <v>4637733017.055322</v>
+        <v>7182687930.6046</v>
       </c>
       <c r="E75" t="n">
-        <v>0.002257239628741936</v>
+        <v>0.001746550265105777</v>
       </c>
       <c r="F75" t="n">
-        <v>0.3208062030583794</v>
+        <v>0.144413686077085</v>
       </c>
       <c r="G75" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H75" t="n">
-        <v>0.7437417389146614</v>
+        <v>0.2304076399031841</v>
       </c>
       <c r="I75" t="n">
-        <v>568</v>
+        <v>1</v>
+      </c>
+      <c r="J75" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="76">
@@ -2779,25 +3006,28 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>444</v>
+        <v>603</v>
       </c>
       <c r="D76" t="n">
-        <v>4388967488.408028</v>
+        <v>8532947242.039564</v>
       </c>
       <c r="E76" t="n">
-        <v>0.001551751745503338</v>
+        <v>0.002500517279637018</v>
       </c>
       <c r="F76" t="n">
-        <v>0.2649846833159952</v>
+        <v>0.1851051137663505</v>
       </c>
       <c r="G76" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H76" t="n">
-        <v>0.557077094113836</v>
+        <v>0.3689307977591891</v>
       </c>
       <c r="I76" t="n">
-        <v>444</v>
+        <v>1</v>
+      </c>
+      <c r="J76" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="77">
@@ -2810,25 +3040,28 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>520</v>
+        <v>459</v>
       </c>
       <c r="D77" t="n">
-        <v>10699721339.17369</v>
+        <v>12893739993.16342</v>
       </c>
       <c r="E77" t="n">
-        <v>0.003583660996018748</v>
+        <v>0.001640206356068186</v>
       </c>
       <c r="F77" t="n">
-        <v>0.127300773246604</v>
+        <v>0.09324680121031517</v>
       </c>
       <c r="G77" t="b">
         <v>0</v>
       </c>
       <c r="H77" t="n">
-        <v>0.09666830756520273</v>
+        <v>0.05622357038553062</v>
       </c>
       <c r="I77" t="n">
-        <v>520</v>
+        <v>1</v>
+      </c>
+      <c r="J77" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="78">
@@ -2841,25 +3074,28 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>478</v>
+        <v>458</v>
       </c>
       <c r="D78" t="n">
-        <v>4884551540.283016</v>
+        <v>8443449402.783299</v>
       </c>
       <c r="E78" t="n">
-        <v>0.002291478011280351</v>
+        <v>0.002681387335630043</v>
       </c>
       <c r="F78" t="n">
-        <v>0.256332318263849</v>
+        <v>0.1420841841729444</v>
       </c>
       <c r="G78" t="b">
         <v>0</v>
       </c>
       <c r="H78" t="n">
-        <v>0.5281439755495337</v>
+        <v>0.222477469390188</v>
       </c>
       <c r="I78" t="n">
-        <v>478</v>
+        <v>1</v>
+      </c>
+      <c r="J78" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="79">
@@ -2872,25 +3108,28 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>425</v>
+        <v>533</v>
       </c>
       <c r="D79" t="n">
-        <v>10877591875.5567</v>
+        <v>6035688956.6077</v>
       </c>
       <c r="E79" t="n">
-        <v>0.003928845664380482</v>
+        <v>0.002286660564860322</v>
       </c>
       <c r="F79" t="n">
-        <v>0.1023425738652311</v>
+        <v>0.2313132568688039</v>
       </c>
       <c r="G79" t="b">
         <v>0</v>
       </c>
       <c r="H79" t="n">
-        <v>0.01320921429987176</v>
+        <v>0.526234147990437</v>
       </c>
       <c r="I79" t="n">
-        <v>425</v>
+        <v>1</v>
+      </c>
+      <c r="J79" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="80">
@@ -2903,25 +3142,28 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>462</v>
+        <v>562</v>
       </c>
       <c r="D80" t="n">
-        <v>10221795319.45441</v>
+        <v>5101189513.504308</v>
       </c>
       <c r="E80" t="n">
-        <v>0.002232241306376718</v>
+        <v>0.00240263065359294</v>
       </c>
       <c r="F80" t="n">
-        <v>0.1183899835772286</v>
+        <v>0.2885791982640397</v>
       </c>
       <c r="G80" t="b">
         <v>0</v>
       </c>
       <c r="H80" t="n">
-        <v>0.06687102873429523</v>
+        <v>0.7211808355395112</v>
       </c>
       <c r="I80" t="n">
-        <v>462</v>
+        <v>1</v>
+      </c>
+      <c r="J80" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="81">
@@ -2934,25 +3176,28 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>424</v>
+        <v>387</v>
       </c>
       <c r="D81" t="n">
-        <v>9590908621.123678</v>
+        <v>3410424528.998973</v>
       </c>
       <c r="E81" t="n">
-        <v>0.001917182933926802</v>
+        <v>0.001780150818363885</v>
       </c>
       <c r="F81" t="n">
-        <v>0.115799389179237</v>
+        <v>0.2972368751691867</v>
       </c>
       <c r="G81" t="b">
         <v>0</v>
       </c>
       <c r="H81" t="n">
-        <v>0.05820819788777229</v>
+        <v>0.7506535970694375</v>
       </c>
       <c r="I81" t="n">
-        <v>424</v>
+        <v>1</v>
+      </c>
+      <c r="J81" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="82">
@@ -2965,25 +3210,28 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>438</v>
+        <v>496</v>
       </c>
       <c r="D82" t="n">
-        <v>7328728345.474451</v>
+        <v>11329208637.06666</v>
       </c>
       <c r="E82" t="n">
-        <v>0.003206823848763001</v>
+        <v>0.003856824950587691</v>
       </c>
       <c r="F82" t="n">
-        <v>0.1565473252543823</v>
+        <v>0.1146785694941877</v>
       </c>
       <c r="G82" t="b">
         <v>0</v>
       </c>
       <c r="H82" t="n">
-        <v>0.1944674586340988</v>
+        <v>0.1291823331940268</v>
       </c>
       <c r="I82" t="n">
-        <v>438</v>
+        <v>1</v>
+      </c>
+      <c r="J82" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="83">
@@ -2996,25 +3244,28 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>437</v>
+        <v>568</v>
       </c>
       <c r="D83" t="n">
-        <v>8296185446.883107</v>
+        <v>6422855426.036601</v>
       </c>
       <c r="E83" t="n">
-        <v>0.001812576781077812</v>
+        <v>0.001074467946424377</v>
       </c>
       <c r="F83" t="n">
-        <v>0.137975873047782</v>
+        <v>0.2316436259749499</v>
       </c>
       <c r="G83" t="b">
         <v>0</v>
       </c>
       <c r="H83" t="n">
-        <v>0.1323653599169904</v>
+        <v>0.5273588018657172</v>
       </c>
       <c r="I83" t="n">
-        <v>437</v>
+        <v>1</v>
+      </c>
+      <c r="J83" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="84">
@@ -3027,25 +3278,28 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>526</v>
+        <v>605</v>
       </c>
       <c r="D84" t="n">
-        <v>3914849555.869042</v>
+        <v>8468665402.077128</v>
       </c>
       <c r="E84" t="n">
-        <v>0.001655168646819171</v>
+        <v>0.002189648524973373</v>
       </c>
       <c r="F84" t="n">
-        <v>0.3519417848214471</v>
+        <v>0.1871287711533992</v>
       </c>
       <c r="G84" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H84" t="n">
-        <v>0.8478577203012666</v>
+        <v>0.3758198018465676</v>
       </c>
       <c r="I84" t="n">
-        <v>526</v>
+        <v>1</v>
+      </c>
+      <c r="J84" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="85">
@@ -3058,25 +3312,28 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="D85" t="n">
-        <v>9236913365.875135</v>
+        <v>12087850012.67897</v>
       </c>
       <c r="E85" t="n">
-        <v>0.002764320414065716</v>
+        <v>0.002715974243362818</v>
       </c>
       <c r="F85" t="n">
-        <v>0.1369684135691939</v>
+        <v>0.1040141297816574</v>
       </c>
       <c r="G85" t="b">
         <v>0</v>
       </c>
       <c r="H85" t="n">
-        <v>0.1289964608510074</v>
+        <v>0.09287808068596387</v>
       </c>
       <c r="I85" t="n">
-        <v>483</v>
+        <v>1</v>
+      </c>
+      <c r="J85" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="86">
@@ -3089,25 +3346,28 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>514</v>
+        <v>589</v>
       </c>
       <c r="D86" t="n">
-        <v>10121567626.59756</v>
+        <v>10092559107.29406</v>
       </c>
       <c r="E86" t="n">
-        <v>0.003747675497186098</v>
+        <v>0.001306615275381153</v>
       </c>
       <c r="F86" t="n">
-        <v>0.1330195587946282</v>
+        <v>0.1528671463400177</v>
       </c>
       <c r="G86" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H86" t="n">
-        <v>0.1157916685546653</v>
+        <v>0.2591852001149781</v>
       </c>
       <c r="I86" t="n">
-        <v>514</v>
+        <v>1</v>
+      </c>
+      <c r="J86" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="87">
@@ -3120,25 +3380,28 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>415</v>
+        <v>594</v>
       </c>
       <c r="D87" t="n">
-        <v>10044607460.09065</v>
+        <v>9838091705.12961</v>
       </c>
       <c r="E87" t="n">
-        <v>0.00213187991332115</v>
+        <v>0.001730716117933279</v>
       </c>
       <c r="F87" t="n">
-        <v>0.108221934437863</v>
+        <v>0.1581523842869588</v>
       </c>
       <c r="G87" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H87" t="n">
-        <v>0.03286953093064617</v>
+        <v>0.2771773889371906</v>
       </c>
       <c r="I87" t="n">
-        <v>415</v>
+        <v>1</v>
+      </c>
+      <c r="J87" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="88">
@@ -3151,25 +3414,28 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>449</v>
+        <v>442</v>
       </c>
       <c r="D88" t="n">
-        <v>3828905445.803045</v>
+        <v>4442206356.621651</v>
       </c>
       <c r="E88" t="n">
-        <v>0.004376081163326431</v>
+        <v>0.003298927118167436</v>
       </c>
       <c r="F88" t="n">
-        <v>0.3071650963042605</v>
+        <v>0.2606295806754231</v>
       </c>
       <c r="G88" t="b">
         <v>0</v>
       </c>
       <c r="H88" t="n">
-        <v>0.6981264930614682</v>
+        <v>0.6260337859248263</v>
       </c>
       <c r="I88" t="n">
-        <v>449</v>
+        <v>1</v>
+      </c>
+      <c r="J88" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="89">
@@ -3182,25 +3448,28 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>509</v>
+        <v>578</v>
       </c>
       <c r="D89" t="n">
-        <v>5753978584.41018</v>
+        <v>4107504592.450338</v>
       </c>
       <c r="E89" t="n">
-        <v>0.002511555927821913</v>
+        <v>0.001280075440552624</v>
       </c>
       <c r="F89" t="n">
-        <v>0.2317126298683763</v>
+        <v>0.36859542963939</v>
       </c>
       <c r="G89" t="b">
         <v>0</v>
       </c>
       <c r="H89" t="n">
-        <v>0.4458168477562261</v>
+        <v>0.993574842810342</v>
       </c>
       <c r="I89" t="n">
-        <v>509</v>
+        <v>1</v>
+      </c>
+      <c r="J89" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="90">
@@ -3213,25 +3482,28 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>456</v>
+        <v>431</v>
       </c>
       <c r="D90" t="n">
-        <v>9669908945.450256</v>
+        <v>6390894406.951451</v>
       </c>
       <c r="E90" t="n">
-        <v>0.00104923938025695</v>
+        <v>0.003534428900257333</v>
       </c>
       <c r="F90" t="n">
-        <v>0.1235215188413942</v>
+        <v>0.1766508751532524</v>
       </c>
       <c r="G90" t="b">
         <v>0</v>
       </c>
       <c r="H90" t="n">
-        <v>0.08403065125602101</v>
+        <v>0.3401505878609885</v>
       </c>
       <c r="I90" t="n">
-        <v>456</v>
+        <v>1</v>
+      </c>
+      <c r="J90" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="91">
@@ -3244,25 +3516,28 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>481</v>
+        <v>454</v>
       </c>
       <c r="D91" t="n">
-        <v>7196983839.078497</v>
+        <v>4651875114.66156</v>
       </c>
       <c r="E91" t="n">
-        <v>0.001304259300510288</v>
+        <v>0.001962726968511287</v>
       </c>
       <c r="F91" t="n">
-        <v>0.1750631400835994</v>
+        <v>0.2556395067984362</v>
       </c>
       <c r="G91" t="b">
         <v>0</v>
       </c>
       <c r="H91" t="n">
-        <v>0.2563835084701516</v>
+        <v>0.6090464047826958</v>
       </c>
       <c r="I91" t="n">
-        <v>481</v>
+        <v>1</v>
+      </c>
+      <c r="J91" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="92">
@@ -3275,25 +3550,28 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>549</v>
+        <v>379</v>
       </c>
       <c r="D92" t="n">
-        <v>9036396874.800261</v>
+        <v>9525447260.450104</v>
       </c>
       <c r="E92" t="n">
-        <v>0.004153207347415489</v>
+        <v>0.002117266920926892</v>
       </c>
       <c r="F92" t="n">
-        <v>0.1591392155440037</v>
+        <v>0.1042207030132767</v>
       </c>
       <c r="G92" t="b">
         <v>0</v>
       </c>
       <c r="H92" t="n">
-        <v>0.2031346228837947</v>
+        <v>0.09358130438681141</v>
       </c>
       <c r="I92" t="n">
-        <v>549</v>
+        <v>1</v>
+      </c>
+      <c r="J92" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="93">
@@ -3306,25 +3584,28 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>481</v>
+        <v>396</v>
       </c>
       <c r="D93" t="n">
-        <v>7512216172.317144</v>
+        <v>11172889320.85979</v>
       </c>
       <c r="E93" t="n">
-        <v>0.003862009272679614</v>
+        <v>0.001482920202852919</v>
       </c>
       <c r="F93" t="n">
-        <v>0.1677170306470794</v>
+        <v>0.09283887186310889</v>
       </c>
       <c r="G93" t="b">
         <v>0</v>
       </c>
       <c r="H93" t="n">
-        <v>0.2318184497801635</v>
+        <v>0.05483488326969223</v>
       </c>
       <c r="I93" t="n">
-        <v>481</v>
+        <v>1</v>
+      </c>
+      <c r="J93" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="94">
@@ -3337,25 +3618,28 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>454</v>
+        <v>512</v>
       </c>
       <c r="D94" t="n">
-        <v>4506914174.353644</v>
+        <v>7420208349.970246</v>
       </c>
       <c r="E94" t="n">
-        <v>0.004689348671871648</v>
+        <v>0.001073756052684995</v>
       </c>
       <c r="F94" t="n">
-        <v>0.2638619272510439</v>
+        <v>0.1807398952625606</v>
       </c>
       <c r="G94" t="b">
         <v>0</v>
       </c>
       <c r="H94" t="n">
-        <v>0.5533226484622431</v>
+        <v>0.354070570772463</v>
       </c>
       <c r="I94" t="n">
-        <v>454</v>
+        <v>1</v>
+      </c>
+      <c r="J94" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="95">
@@ -3368,25 +3652,28 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>583</v>
+        <v>504</v>
       </c>
       <c r="D95" t="n">
-        <v>8974709833.452888</v>
+        <v>5992382979.312372</v>
       </c>
       <c r="E95" t="n">
-        <v>0.001191019939142208</v>
+        <v>0.002183530205805787</v>
       </c>
       <c r="F95" t="n">
-        <v>0.1701564059829296</v>
+        <v>0.2203084423271441</v>
       </c>
       <c r="G95" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H95" t="n">
-        <v>0.2399756109019635</v>
+        <v>0.4887711797807337</v>
       </c>
       <c r="I95" t="n">
-        <v>583</v>
+        <v>1</v>
+      </c>
+      <c r="J95" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="96">
@@ -3399,25 +3686,28 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>595</v>
+        <v>578</v>
       </c>
       <c r="D96" t="n">
-        <v>6641108333.945624</v>
+        <v>13917092155.18392</v>
       </c>
       <c r="E96" t="n">
-        <v>0.002045385215249732</v>
+        <v>0.003703972865183998</v>
       </c>
       <c r="F96" t="n">
-        <v>0.2346802629364788</v>
+        <v>0.1087876262597035</v>
       </c>
       <c r="G96" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H96" t="n">
-        <v>0.4557404789134039</v>
+        <v>0.109128181596724</v>
       </c>
       <c r="I96" t="n">
-        <v>595</v>
+        <v>1</v>
+      </c>
+      <c r="J96" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="97">
@@ -3430,25 +3720,28 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>599</v>
+        <v>580</v>
       </c>
       <c r="D97" t="n">
-        <v>4450801484.109453</v>
+        <v>5773967801.898241</v>
       </c>
       <c r="E97" t="n">
-        <v>0.003263687175329887</v>
+        <v>0.001835714537144573</v>
       </c>
       <c r="F97" t="n">
-        <v>0.3525240601275523</v>
+        <v>0.263119963970103</v>
       </c>
       <c r="G97" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H97" t="n">
-        <v>0.8498048226677382</v>
+        <v>0.6345116344015437</v>
       </c>
       <c r="I97" t="n">
-        <v>599</v>
+        <v>1</v>
+      </c>
+      <c r="J97" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="98">
@@ -3461,25 +3754,28 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>408</v>
+        <v>423</v>
       </c>
       <c r="D98" t="n">
-        <v>5966604384.674321</v>
+        <v>4071688298.241373</v>
       </c>
       <c r="E98" t="n">
-        <v>0.001715347788404721</v>
+        <v>0.001755445146982878</v>
       </c>
       <c r="F98" t="n">
-        <v>0.1791154651957596</v>
+        <v>0.2721234752862993</v>
       </c>
       <c r="G98" t="b">
         <v>0</v>
       </c>
       <c r="H98" t="n">
-        <v>0.2699343009095145</v>
+        <v>0.6651616973296821</v>
       </c>
       <c r="I98" t="n">
-        <v>408</v>
+        <v>1</v>
+      </c>
+      <c r="J98" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="99">
@@ -3492,25 +3788,28 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>533</v>
+        <v>417</v>
       </c>
       <c r="D99" t="n">
-        <v>5965481524.311284</v>
+        <v>10573149157.03197</v>
       </c>
       <c r="E99" t="n">
-        <v>0.004233064340437886</v>
+        <v>0.004987218711569141</v>
       </c>
       <c r="F99" t="n">
-        <v>0.2340355701899829</v>
+        <v>0.1033075022188205</v>
       </c>
       <c r="G99" t="b">
         <v>0</v>
       </c>
       <c r="H99" t="n">
-        <v>0.4535846554409206</v>
+        <v>0.09047255482976271</v>
       </c>
       <c r="I99" t="n">
-        <v>533</v>
+        <v>1</v>
+      </c>
+      <c r="J99" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="100">
@@ -3523,25 +3822,28 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>445</v>
+        <v>502</v>
       </c>
       <c r="D100" t="n">
-        <v>5425656682.712706</v>
+        <v>6343044377.480233</v>
       </c>
       <c r="E100" t="n">
-        <v>0.001900736546156981</v>
+        <v>0.002270177291117059</v>
       </c>
       <c r="F100" t="n">
-        <v>0.2148364001198123</v>
+        <v>0.2073032603505694</v>
       </c>
       <c r="G100" t="b">
         <v>0</v>
       </c>
       <c r="H100" t="n">
-        <v>0.3893834964943658</v>
+        <v>0.4444984919398402</v>
       </c>
       <c r="I100" t="n">
-        <v>445</v>
+        <v>1</v>
+      </c>
+      <c r="J100" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="101">
@@ -3554,25 +3856,28 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>649</v>
+        <v>604</v>
       </c>
       <c r="D101" t="n">
-        <v>7758617419.165174</v>
+        <v>11753776985.38624</v>
       </c>
       <c r="E101" t="n">
-        <v>0.004566768039588344</v>
+        <v>0.003169170035935485</v>
       </c>
       <c r="F101" t="n">
-        <v>0.21910915542771</v>
+        <v>0.1346045243130849</v>
       </c>
       <c r="G101" t="b">
         <v>1</v>
       </c>
       <c r="H101" t="n">
-        <v>0.4036713975681874</v>
+        <v>0.1970149540076206</v>
       </c>
       <c r="I101" t="n">
-        <v>649</v>
+        <v>1</v>
+      </c>
+      <c r="J101" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>